<commit_message>
Replace doc-pol_new.xlsx with Spanish version
</commit_message>
<xml_diff>
--- a/tools/excel/intuitem/doc-pol_new.xlsx
+++ b/tools/excel/intuitem/doc-pol_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ciso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thidalgo.INDRA\OneDrive - Indra\Documentos\CISO_ASSISTANT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B9D3A5-D92B-4699-B0E0-179179FCBE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAEFAC6-EA65-4123-B562-35BECC95C9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="747" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="854">
   <si>
     <t>type</t>
   </si>
@@ -2762,6 +2762,709 @@
 Retention rules
 Use of test information
 Continual improvement</t>
+  </si>
+  <si>
+    <t>name[es]</t>
+  </si>
+  <si>
+    <t>description[es]</t>
+  </si>
+  <si>
+    <t>Documentación, políticas, procedimientos, formación y controles técnicos habituales recomendados por Intuitem</t>
+  </si>
+  <si>
+    <t>Documento de visión general de la organización</t>
+  </si>
+  <si>
+    <t>Documento de contexto de la organización</t>
+  </si>
+  <si>
+    <t>Documento de alcance del SGSI</t>
+  </si>
+  <si>
+    <t>Registro legal</t>
+  </si>
+  <si>
+    <t>Documento de declaración de aplicabilidad</t>
+  </si>
+  <si>
+    <t>Matriz de responsabilidad de los controles</t>
+  </si>
+  <si>
+    <t>Documento del plan de auditoría</t>
+  </si>
+  <si>
+    <t>Matriz de competencias</t>
+  </si>
+  <si>
+    <t>Matriz de responsabilidades</t>
+  </si>
+  <si>
+    <t>Documento del plan de comunicación</t>
+  </si>
+  <si>
+    <t>Registro de riesgos</t>
+  </si>
+  <si>
+    <t>Registro de objetivos de seguridad</t>
+  </si>
+  <si>
+    <t>Documento del plan de revisión por la dirección</t>
+  </si>
+  <si>
+    <t>Registro de formación y concienciación</t>
+  </si>
+  <si>
+    <t>Registro de documentos</t>
+  </si>
+  <si>
+    <t>Registro de procedimientos operativos</t>
+  </si>
+  <si>
+    <t>Registro de no conformidades</t>
+  </si>
+  <si>
+    <t>Documento de normas de funcionamiento</t>
+  </si>
+  <si>
+    <t>Registro de activos</t>
+  </si>
+  <si>
+    <t>Registro de proveedores</t>
+  </si>
+  <si>
+    <t>Plan de concienciación y formación en seguridad de la información</t>
+  </si>
+  <si>
+    <t>Plan de aseguramiento de la seguridad</t>
+  </si>
+  <si>
+    <t>Mapa del sistema de información</t>
+  </si>
+  <si>
+    <t>Registro de cuentas de acceso privilegiado</t>
+  </si>
+  <si>
+    <t>Registro de incidentes de seguridad</t>
+  </si>
+  <si>
+    <t>Matriz de flujos</t>
+  </si>
+  <si>
+    <t>Principios de arquitectura de seguridad</t>
+  </si>
+  <si>
+    <t>Objetivos de la organización
+Organigrama
+Objetivos del SGSI
+Responsabilidades del CISO
+Revisión del SGSI por la dirección</t>
+  </si>
+  <si>
+    <t>Partes interesadas
+Autoridades
+Grupos de interés especial</t>
+  </si>
+  <si>
+    <t>Productos y servicios
+Productos y servicios que requieren certificación
+Ubicaciones
+Vista de la organización
+Vista de la arquitectura de negocio
+Vista de la arquitectura de datos
+Vista de la arquitectura de aplicaciones
+Vista de la arquitectura tecnológica
+Vista de la red
+Declaración de alcance</t>
+  </si>
+  <si>
+    <t>Requisitos legales
+Requisitos estatutarios
+Requisitos reglamentarios
+Requisitos contractuales
+Derechos de propiedad intelectual
+Contratos laborales
+Acuerdos de confidencialidad</t>
+  </si>
+  <si>
+    <t>Contexto de la organización
+Liderazgo
+Planificación
+Soporte
+Operación
+Evaluación del desempeño
+Mejora
+Controles organizativos
+Controles de las personas
+Controles físicos
+Controles tecnológicos</t>
+  </si>
+  <si>
+    <t>RACI para el SGSI</t>
+  </si>
+  <si>
+    <t>Propietario del riesgo
+Impacto
+Probabilidad
+Nivel de riesgo
+Evaluación
+Prioridad
+Opción de tratamiento
+Mitigaciones – medidas de seguridad recomendadas</t>
+  </si>
+  <si>
+    <t>Revisión de riesgos
+Revisión de los objetivos de seguridad
+Revisión de los incidentes de seguridad
+Revisión de la gestión de vulnerabilidades
+Revisión de las no conformidades</t>
+  </si>
+  <si>
+    <t>Normas para la edición y el mantenimiento
+Control de versiones
+Registro
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Lista de no conformidades (incidentes, problemas, …)
+Acción correctiva adoptada</t>
+  </si>
+  <si>
+    <t>Gestión de riesgos</t>
+  </si>
+  <si>
+    <t>Objetivo: Sensibilizar a todos los empleados y proporcionar formación específica al personal pertinente para promover comportamientos seguros, garantizar el cumplimiento y reducir los riesgos.
+Alcance: Concienciación para todos los empleados y contratistas; formación específica para determinados equipos (por ejemplo, TI, seguridad, gestores de accesos).
+Funciones y responsabilidades: Asignar responsabilidades a los equipos de TI, RR. HH. y seguridad.
+Requisitos de formación: Definir los contenidos obligatorios (por ejemplo, gestión de accesos, configuraciones seguras) y la periodicidad (por ejemplo, anual, incorporación).
+Métodos de impartición: Concienciación mediante formación en línea y campañas; formación mediante talleres prácticos y simulaciones.
+Evaluación: Realizar el seguimiento de las tasas de participación, los resultados de los cuestionarios y los resultados de las pruebas de phishing.
+Cumplimiento: Alinear con la normativa (por ejemplo, RGPD, ISO 27001) y mantener registros preparados para auditoría.
+Mejora continua: Actualizar en función de la retroalimentación y de las amenazas emergentes.</t>
+  </si>
+  <si>
+    <t>Documento proporcionado por los proveedores que describe las medidas de seguridad, el cumplimiento de normas (por ejemplo, ISO 27001) y los procedimientos de prueba para garantizar la seguridad de sus productos, servicios o sistemas. Demuestra su compromiso con el mantenimiento de un entorno seguro y proporciona evidencias de cumplimiento y de las prácticas de seguridad.</t>
+  </si>
+  <si>
+    <t>Representación visual de los componentes del sistema de información de una organización y de sus interacciones para mejorar su gestión y seguridad.</t>
+  </si>
+  <si>
+    <t>Documento que mapea los flujos de datos autorizados entre sistemas, aplicaciones o zonas de red para garantizar una comunicación segura y conforme a los requisitos.</t>
+  </si>
+  <si>
+    <t>Procedimiento de gestión de accesos privilegiados</t>
+  </si>
+  <si>
+    <t>Procedimiento de recertificación de cuentas</t>
+  </si>
+  <si>
+    <t>Procedimiento de seguridad física</t>
+  </si>
+  <si>
+    <t>Procedimiento de objetos de directiva de grupo</t>
+  </si>
+  <si>
+    <t>Procedimiento de gestión de actualizaciones</t>
+  </si>
+  <si>
+    <t>Procedimiento de gestión de incidentes</t>
+  </si>
+  <si>
+    <t>Procedimiento de eliminación segura</t>
+  </si>
+  <si>
+    <t>Procedimiento de sincronización horaria</t>
+  </si>
+  <si>
+    <t>Procedimiento de configuración de la seguridad del correo electrónico</t>
+  </si>
+  <si>
+    <t>Procedimiento de registro de eventos</t>
+  </si>
+  <si>
+    <t>Procedimiento de seguridad de RR.HH.</t>
+  </si>
+  <si>
+    <t>Documento que describe los procesos y controles para la gestión y protección de las cuentas privilegiadas, garantizando que únicamente los usuarios autorizados tengan acceso a los sistemas y datos críticos, mediante medidas como la monitorización, la auditoría y el acceso con tiempo limitado para minimizar los riesgos.</t>
+  </si>
+  <si>
+    <t>Documento que define el proceso para la revisión y validación periódicas de los derechos de acceso de los usuarios, las certificaciones de los sistemas o el cumplimiento de normas. Garantiza que solo los usuarios y sistemas autorizados mantengan el acceso o la certificación, y ayuda a identificar y revocar permisos obsoletos o innecesarios.</t>
+  </si>
+  <si>
+    <t>Documento que describe los procesos y controles relacionados con la gestión de los recursos humanos dentro de una organización, garantizando el cumplimiento de los requisitos legales, reglamentarios y de seguridad. Incluye los procedimientos de selección, incorporación, cambios de puesto, formación y finalización de la relación laboral para proteger la información y los activos de la organización.</t>
+  </si>
+  <si>
+    <t>Documento que define cómo crear, configurar y gestionar los GPO para aplicar ajustes de seguridad, configuraciones del sistema y políticas de usuario en un entorno Windows. Garantiza la aplicación coherente de las políticas organizativas para unas operaciones de TI seguras y conformes.</t>
+  </si>
+  <si>
+    <t>Control de accesos: Procedimientos para conceder, revocar y supervisar el acceso físico a las áreas seguras.
+Protección de activos: Directrices para la protección de los activos críticos (por ejemplo, servidores, dispositivos de almacenamiento).
+Vigilancia: Uso de cámaras, alarmas y sistemas de monitorización para detectar y prevenir intrusiones.
+Gestión de visitantes: Políticas para el registro y el acompañamiento de visitantes en áreas seguras.
+Respuesta ante incidentes: Pasos para abordar brechas de seguridad física o situaciones de emergencia.</t>
+  </si>
+  <si>
+    <t>Funciones y responsabilidades
+Clasificación de las actualizaciones
+Planificación de las actualizaciones
+Pruebas y validación
+Proceso de despliegue
+Supervisión y verificación
+Documentación y elaboración de informes</t>
+  </si>
+  <si>
+    <t>Implementación práctica de la política de gestión de incidentes</t>
+  </si>
+  <si>
+    <t>Funciones y responsabilidades
+Identificación de activos para su eliminación
+Métodos de eliminación segura
+Saneado de datos
+Cumplimiento de los requisitos legales y reglamentarios
+Documentación y mantenimiento de registros
+Verificación y auditoría</t>
+  </si>
+  <si>
+    <t>Fuente horaria: Uso de fuentes externas fiables (por ejemplo, servidores NTP).
+Configuración: Definición de intervalos de sincronización y mecanismos de respaldo.
+Supervisión: Verificación periódica del estado de la sincronización horaria.</t>
+  </si>
+  <si>
+    <t>Configuración del servidor de correo electrónico
+Protección del correo electrónico basada en dominios
+Controles antimalware y antispam
+Cifrado y comunicaciones seguras
+Control de accesos y monitorización
+Copia de seguridad y recuperación
+Concienciación y formación de los usuarios</t>
+  </si>
+  <si>
+    <t>Recogida y categorización de registros
+Políticas de almacenamiento seguro y conservación
+Análisis para la detección de anomalías y la respuesta a incidentes</t>
+  </si>
+  <si>
+    <t>Política principal</t>
+  </si>
+  <si>
+    <t>Política de concienciación y formación en seguridad de la información</t>
+  </si>
+  <si>
+    <t>Política de puestos de trabajo y teletrabajo</t>
+  </si>
+  <si>
+    <t>Política criptográfica</t>
+  </si>
+  <si>
+    <t>Política de clasificación y tratamiento de la información</t>
+  </si>
+  <si>
+    <t>Política de auditoría interna y externa</t>
+  </si>
+  <si>
+    <t>Política de continuidad de negocio</t>
+  </si>
+  <si>
+    <t>Política de segregación de funciones</t>
+  </si>
+  <si>
+    <t>Política de control de accesos</t>
+  </si>
+  <si>
+    <t>Política de protección frente a malware</t>
+  </si>
+  <si>
+    <t>Política de gestión de riesgos</t>
+  </si>
+  <si>
+    <t>Política de gestión de activos</t>
+  </si>
+  <si>
+    <t>Política de copia de seguridad y restauración</t>
+  </si>
+  <si>
+    <t>Política de seguridad de proveedores externos</t>
+  </si>
+  <si>
+    <t>Política de registro y monitorización</t>
+  </si>
+  <si>
+    <t>Política de transferencia de la información</t>
+  </si>
+  <si>
+    <t>Política de desarrollo seguro</t>
+  </si>
+  <si>
+    <t>Política de seguridad física</t>
+  </si>
+  <si>
+    <t>Política de gestión de la seguridad de red</t>
+  </si>
+  <si>
+    <t>Política de uso aceptable</t>
+  </si>
+  <si>
+    <t>Política de integración de proyectos de sistemas de información</t>
+  </si>
+  <si>
+    <t>Política de inteligencia de amenazas</t>
+  </si>
+  <si>
+    <t>Política de gestión de incidentes de seguridad de la información</t>
+  </si>
+  <si>
+    <t>Política de mantenimiento</t>
+  </si>
+  <si>
+    <t>Política de gestión de vulnerabilidades</t>
+  </si>
+  <si>
+    <t>Objetivos de seguridad de la información
+Compromiso
+Revisión por la dirección
+Políticas aplicables
+Gestión de las no conformidades
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Implicaciones del incumplimiento
+Notificación de eventos de seguridad
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Puestos de trabajo
+Dispositivos móviles
+Teletrabajo
+Gestión de contraseñas
+Devolución de activos
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Gestión de claves
+Cifrado
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Clasificación
+Protección y tratamiento de la información
+Protección y tratamiento de los datos personales
+Mesa limpia
+Pantalla limpia
+Protección de los registros
+Normas de conservación
+Uso de información de prueba
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Protección de la información de auditoría</t>
+  </si>
+  <si>
+    <t>Identificación
+Autenticación
+Gestión de contraseñas
+RBAC (control de acceso basado en roles)
+Revisión de los derechos de acceso
+Aprovisionamiento
+Bajas de usuarios
+Acceso remoto
+Gestión de accesos privilegiados
+Acceso de terceros
+Supervisión y elaboración de informes
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Antivirus
+EDR</t>
+  </si>
+  <si>
+    <t>Definición de la gestión de riesgos
+Apetito de riesgo
+Criterios de aceptación del riesgo
+Criterios para la evaluación de riesgos
+Identificación de riesgos
+Evaluación de riesgos
+Enfoque CIAP
+Informes de riesgos
+Revisión de riesgos
+Tratamiento del riesgo (mitigación, aceptación, transferencia)
+Evaluación del riesgo
+Uso de los controles de la ISO/IEC 27002
+Gestión de los derechos de acceso
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Registro de eventos</t>
+  </si>
+  <si>
+    <t>Perímetro de seguridad física
+Áreas seguras
+Control de acceso de empleados
+Control de acceso de visitantes
+Gestión de entregas
+Seguridad del cableado
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Objetivo: Definir los usos permitidos y prohibidos de los recursos.
+Alcance: Todos los usuarios de los sistemas de información.
+Normas: Actividades permitidas y prohibidas, obligaciones de seguridad.
+Confidencialidad: Protección de los datos sensibles.
+Cumplimiento: Supervisión y sanciones por incumplimiento.</t>
+  </si>
+  <si>
+    <t>Normas para la integración de la seguridad en los proyectos de sistemas de información</t>
+  </si>
+  <si>
+    <t>Vulnerabilidades conocidas explotadas
+Actividad de actores de amenazas
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Clasificación de incidentes
+Notificación de incidentes
+Proceso de respuesta a incidentes
+Análisis de la causa raíz y lecciones aprendidas
+Documentación y comunicación
+Funciones y responsabilidades
+Revisión y actualización</t>
+  </si>
+  <si>
+    <t>Gestión de la obsolescencia
+Contratos de mantenimiento
+Gestión de cambios</t>
+  </si>
+  <si>
+    <t>Detección y gestión de vulnerabilidades
+Gestión de parches</t>
+  </si>
+  <si>
+    <t>Formación en requisitos legales y reglamentarios</t>
+  </si>
+  <si>
+    <t>Formación sobre el panorama de amenazas</t>
+  </si>
+  <si>
+    <t>Formación en IAM (gestión de identidades y accesos)</t>
+  </si>
+  <si>
+    <t>Formación en seguridad de red</t>
+  </si>
+  <si>
+    <t>Formación en mantenimiento de condiciones de seguridad (SCM)</t>
+  </si>
+  <si>
+    <t>Formación en registro y monitorización</t>
+  </si>
+  <si>
+    <t>Registro de accesos</t>
+  </si>
+  <si>
+    <t>Antivirus de host, cortafuegos y control de USB</t>
+  </si>
+  <si>
+    <t>Base de datos de gestión de la configuración (CMDB)</t>
+  </si>
+  <si>
+    <t>Gestión de información y eventos de seguridad (SIEM)</t>
+  </si>
+  <si>
+    <t>Filtro de pantalla</t>
+  </si>
+  <si>
+    <t>Cortafuegos de red</t>
+  </si>
+  <si>
+    <t>Pasarela de correo seguro</t>
+  </si>
+  <si>
+    <t>Antivirus de red</t>
+  </si>
+  <si>
+    <t>Microsegmentación</t>
+  </si>
+  <si>
+    <t>Seguridad Wi-Fi</t>
+  </si>
+  <si>
+    <t>Proxy inverso</t>
+  </si>
+  <si>
+    <t>Cortafuegos de aplicaciones web (WAF)</t>
+  </si>
+  <si>
+    <t>Sistema de detección de intrusiones (IDS)</t>
+  </si>
+  <si>
+    <t>Autenticación multifactor (MFA)</t>
+  </si>
+  <si>
+    <t>Control de acceso a la red (NAC)(802.1X)</t>
+  </si>
+  <si>
+    <t>Formación en bastionado y configuración segura</t>
+  </si>
+  <si>
+    <t>Gestión de contraseñas</t>
+  </si>
+  <si>
+    <t>Gestión unificada de endpoints</t>
+  </si>
+  <si>
+    <t>Cifrado de discos</t>
+  </si>
+  <si>
+    <t>Copias de seguridad inmutables</t>
+  </si>
+  <si>
+    <t>Cifrado de archivos</t>
+  </si>
+  <si>
+    <t>Detección y respuesta de eventos (EDR)</t>
+  </si>
+  <si>
+    <t>Objetivo: Garantizar la concienciación sobre el cumplimiento de los requisitos legales y reglamentarios.
+Destinatarios: Todos los empleados; adaptado a funciones específicas.
+Contenidos: Principales normativas (por ejemplo, RGPD), tratamiento de datos, riesgos del incumplimiento.
+Métodos: Formación en línea, talleres y estudios de casos.
+Evaluación: Cuestionarios y pruebas basadas en escenarios.</t>
+  </si>
+  <si>
+    <t>Objetivo: Comprender las amenazas cibernéticas actuales y las estrategias de mitigación.
+Destinatarios: Personal de TI, equipos de seguridad y responsables de la toma de decisiones.
+Contenidos: Amenazas emergentes, técnicas de ataque y mecanismos de defensa.
+Métodos: Presentaciones, estudios de casos y debates basados en escenarios.
+Resultado: Mayor concienciación y preparación para hacer frente a amenazas en evolución.</t>
+  </si>
+  <si>
+    <t>Objetivo: Comprender y dominar la gestión de identidades y accesos.
+Destinatarios: Administradores de TI, equipos de seguridad y gestores de accesos.
+Contenidos:
+-Conceptos clave (identidad, autenticación, autorización, modelos RBAC/ABAC).
+-Buenas prácticas de IAM (gestión de derechos, aprovisionamiento, auditorías).
+-Normas y herramientas (SAML, OAuth, Active Directory, etc.).
+Métodos: Talleres prácticos, casos de uso y demostraciones.
+Resultado: Mejora de las capacidades para proteger y gestionar los accesos de forma segura y eficiente.</t>
+  </si>
+  <si>
+    <t>Objetivo: Desarrollar la especialización en el mantenimiento de sistemas de TI seguros mediante la monitorización, la gestión de parches, el cumplimiento y la respuesta a incidentes.
+Destinatarios: Profesionales de seguridad de TI, administradores de sistemas, responsables de cumplimiento y equipos de respuesta a incidentes.
+Contenidos:
+-Principios del mantenimiento de la seguridad y su importancia en la ciberseguridad.
+-Herramientas y técnicas de monitorización de la seguridad (por ejemplo, SIEM, IDS).
+-Gestión de parches y configuraciones seguras de los sistemas.
+-Detección de incidentes, planificación de la respuesta y ejecución.
+-Cumplimiento de las políticas de seguridad y de los requisitos normativos.
+Métodos: Laboratorios prácticos, escenarios simulados y estudios de casos sobre el mantenimiento de las condiciones de seguridad.
+Resultado: Mejora de la capacidad para proteger de forma continua los entornos de TI, mitigar riesgos y garantizar el cumplimiento.</t>
+  </si>
+  <si>
+    <t>Objetivo: Enseñar prácticas eficaces de registro de eventos y técnicas de monitorización para reforzar la seguridad y la respuesta a incidentes.
+Destinatarios: Administradores de TI, equipos de seguridad y analistas de SOC.
+Contenidos:
+-Importancia del registro de eventos y de los requisitos de cumplimiento.
+-Configuración y gestión de las fuentes de registro (por ejemplo, servidores, cortafuegos, aplicaciones).
+-Sistemas centralizados de registro de eventos (por ejemplo, SIEM, pila ELK).
+-Detección de anomalías y análisis de registros.
+-Respuesta a incidentes basada en la información obtenida de los registros.
+Métodos: Laboratorios prácticos, escenarios reales y ejercicios de análisis de registros.
+Resultado: Mejora de la capacidad para recopilar, analizar y actuar sobre los datos de registro con el fin de prevenir y responder a incidentes.</t>
+  </si>
+  <si>
+    <t>Objetivo: Dotar a los participantes de los conocimientos necesarios para implementar configuraciones seguras y bastionar los sistemas con el fin de reducir vulnerabilidades.
+Destinatarios: Administradores de TI, ingenieros de sistemas y profesionales de la seguridad.
+Contenidos:
+-Principios del bastionado de sistemas.
+-Bastionado de sistemas operativos (Windows, Linux).
+-Aseguramiento de bases de datos (por ejemplo, MySQL, PostgreSQL).
+-Bastionado de dispositivos de red (cortafuegos, routers, switches).
+-Aplicación de los CIS Benchmarks y de las directrices de la ANSSI.
+-Herramientas de automatización (por ejemplo, Ansible, Puppet, Chef).
+Métodos:
+-Laboratorios prácticos para el bastionado de sistemas operativos y aplicaciones.
+-Estudios de casos sobre fallos de bastionado y soluciones.
+Resultado: Los participantes adquirirán la capacidad de implementar configuraciones seguras y mejorar la resiliencia global de los sistemas.</t>
+  </si>
+  <si>
+    <t>Mecanismo que aplica a la autenticación y la autorización de dispositivos o usuarios antes de conceder el acceso a la red. Garantiza un acceso seguro a redes cableadas e inalámbricas mediante el uso de protocolos como 802.1X y RADIUS para validar credenciales y aplicar políticas de acceso.</t>
+  </si>
+  <si>
+    <t>Soluciones integradas para la protección de los endpoints, que incluyen antivirus, cortafuegos y control de puertos USB.</t>
+  </si>
+  <si>
+    <t>Cifrado completo de disco para puestos de trabajo.</t>
+  </si>
+  <si>
+    <t>Utilidades de cifrado de archivos como 7zip.</t>
+  </si>
+  <si>
+    <t>Repositorio centralizado que almacena y gestiona información sobre los activos de TI, sus configuraciones y sus relaciones, para apoyar una gestión eficaz de los sistemas de información.</t>
+  </si>
+  <si>
+    <t>Sistema que recopila, analiza y correlaciona datos de seguridad procedentes de múltiples fuentes para detectar y responder a amenazas.</t>
+  </si>
+  <si>
+    <t>Filtro físico o digital que limita la visibilidad de la pantalla a usuarios autorizados, reduciendo el riesgo de brechas de seguridad por observación visual.</t>
+  </si>
+  <si>
+    <t>Sistema de seguridad que supervisa y controla el tráfico de red entrante y saliente en función de reglas predefinidas.</t>
+  </si>
+  <si>
+    <t>Sistema que filtra, supervisa y protege las comunicaciones de correo electrónico frente a spam, malware y accesos no autorizados.</t>
+  </si>
+  <si>
+    <t>Protege el tráfico de correo electrónico y web en el perímetro de red frente a malware.</t>
+  </si>
+  <si>
+    <t>Las VLAN aíslan y segmentan el tráfico de red para reforzar la seguridad y optimizar el rendimiento.</t>
+  </si>
+  <si>
+    <t>La microsegmentación es una estrategia de seguridad que crea políticas granulares y contextuales para aislar cargas de trabajo o aplicaciones individuales dentro de una red, limitando el movimiento lateral y conteniendo las brechas de seguridad.</t>
+  </si>
+  <si>
+    <t>La seguridad Wi-Fi garantiza comunicaciones inalámbricas seguras mediante cifrado WPA3 Enterprise, autenticación robusta y mecanismos avanzados de control de acceso. Aunque WPA2 Enterprise sigue siendo aceptable, se recomienda encarecidamente la transición a WPA3 para una mayor seguridad.</t>
+  </si>
+  <si>
+    <t>Un proxy inverso reenvía las solicitudes de los clientes a los servidores backend, mejorando la seguridad, el equilibrio de carga y el rendimiento.</t>
+  </si>
+  <si>
+    <t>Un cortafuegos de aplicaciones web (WAF) protege las aplicaciones web filtrando y supervisando el tráfico HTTP para bloquear actividades maliciosas.</t>
+  </si>
+  <si>
+    <t>Un sistema de detección de intrusiones (IDS) supervisa el tráfico de red para detectar y alertar sobre posibles amenazas de seguridad o actividades no autorizadas.</t>
+  </si>
+  <si>
+    <t>Un proxy web filtra y supervisa el tráfico web, aplica políticas de seguridad y permite la autenticación de usuarios para controlar y proteger el acceso a Internet.</t>
+  </si>
+  <si>
+    <t>Una red privada virtual (VPN) protege la transmisión de datos mediante el cifrado del tráfico utilizando protocolos como IPsec, garantizando la confidencialidad y la protección frente a interceptaciones.</t>
+  </si>
+  <si>
+    <t>La autenticación multifactor (MFA) refuerza la seguridad al requerir dos factores de verificación de categorías diferentes: algo que sabes (por ejemplo, una contraseña), algo que tienes (por ejemplo, un token o un teléfono móvil) y algo que eres (por ejemplo, una huella dactilar o reconocimiento facial).</t>
+  </si>
+  <si>
+    <t>Capacidad que permite la creación, el almacenamiento, la gestión y el uso seguros de contraseñas para sistemas, aplicaciones y cuentas. Reduce el riesgo de accesos no autorizados mediante la aplicación de políticas de contraseñas robustas y garantizando un tratamiento seguro de las credenciales.</t>
+  </si>
+  <si>
+    <t>Capacidad que proporciona el control y la gestión centralizados de todos los endpoints, incluidos equipos de sobremesa, portátiles, dispositivos móviles y dispositivos IoT, a través de una única plataforma. Garantiza una configuración segura, la aplicación de políticas, la gestión de aplicaciones y la monitorización en todo el ecosistema de endpoints de la organización.</t>
+  </si>
+  <si>
+    <t>Capacidad que garantiza que las copias de seguridad no puedan ser modificadas, eliminadas ni sobrescritas, protegiendo la integridad de los datos frente a ransomware y accesos no autorizados.</t>
+  </si>
+  <si>
+    <t>Objetivo: Enseñar las mejores prácticas para asegurar las infraestructuras de red y prevenir amenazas cibernéticas.
+Destinatarios: Administradores de TI, ingenieros de redes y profesionales de la seguridad.
+Contenidos:
+-Principios de segregación de redes.
+-Configuración y supervisión de cortafuegos.
+-Sistemas de detección y prevención de intrusiones (IDS/IPS/NDR).
+-Segmentación de red y control de accesos.
+-Protocolos seguros (por ejemplo, HTTPS, VPN, SSH).
+-Mitigación de amenazas (por ejemplo, DDoS, malware).
+  Métodos: Laboratorios interactivos, simulaciones y ejercicios prácticos.
+  Resultado: Mejora de la capacidad para proteger y supervisar entornos de red.</t>
+  </si>
+  <si>
+    <t>Controles de referencia de uso común</t>
   </si>
 </sst>
 </file>
@@ -2846,7 +3549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2888,9 +3591,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3190,16 +3902,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView zoomScale="180" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="76.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="111.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3223,7 +3935,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3312,6 +4024,22 @@
       </c>
       <c r="B14" t="s">
         <v>524</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>687</v>
+      </c>
+      <c r="B15" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>688</v>
+      </c>
+      <c r="B16" t="s">
+        <v>689</v>
       </c>
     </row>
   </sheetData>
@@ -3329,8 +4057,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3356,17 +4084,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K1" sqref="F1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="70.28515625" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
@@ -3374,9 +4102,11 @@
     <col min="8" max="8" width="73.140625" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
     <col min="10" max="10" width="73.140625" customWidth="1"/>
+    <col min="11" max="11" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5">
+    <row r="1" spans="1:12" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -3389,7 +4119,7 @@
       <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -3398,17 +4128,23 @@
       <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="78.75">
+      <c r="K1" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="78.75">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -3439,8 +4175,14 @@
       <c r="J2" s="5" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="63">
+      <c r="K2" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="63">
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
@@ -3471,8 +4213,14 @@
       <c r="J3" s="5" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="157.5">
+      <c r="K3" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="157.5">
       <c r="A4" s="4" t="s">
         <v>41</v>
       </c>
@@ -3503,8 +4251,14 @@
       <c r="J4" s="5" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="110.25">
+      <c r="K4" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="110.25">
       <c r="A5" s="4" t="s">
         <v>47</v>
       </c>
@@ -3535,8 +4289,14 @@
       <c r="J5" s="5" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75">
+      <c r="K5" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -3555,8 +4315,12 @@
       <c r="I6" s="4" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75">
+      <c r="K6" s="5" t="s">
+        <v>694</v>
+      </c>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75">
       <c r="A7" s="4" t="s">
         <v>56</v>
       </c>
@@ -3578,8 +4342,12 @@
       <c r="I7" s="4" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="173.25">
+      <c r="K7" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" ht="173.25">
       <c r="A8" s="4" t="s">
         <v>60</v>
       </c>
@@ -3610,8 +4378,14 @@
       <c r="J8" s="5" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75">
+      <c r="K8" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75">
       <c r="A9" s="4" t="s">
         <v>66</v>
       </c>
@@ -3633,8 +4407,12 @@
       <c r="I9" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75">
+      <c r="K9" s="5" t="s">
+        <v>697</v>
+      </c>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="4" t="s">
         <v>70</v>
       </c>
@@ -3662,8 +4440,14 @@
       <c r="J10" s="4" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75">
+      <c r="K10" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="4" t="s">
         <v>75</v>
       </c>
@@ -3685,8 +4469,12 @@
       <c r="I11" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="141.75">
+      <c r="K11" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" ht="141.75">
       <c r="A12" s="4" t="s">
         <v>79</v>
       </c>
@@ -3717,8 +4505,14 @@
       <c r="J12" s="5" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75">
+      <c r="K12" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75">
       <c r="A13" s="4" t="s">
         <v>85</v>
       </c>
@@ -3740,8 +4534,12 @@
       <c r="I13" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="78.75">
+      <c r="K13" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" ht="78.75">
       <c r="A14" s="4" t="s">
         <v>89</v>
       </c>
@@ -3772,8 +4570,14 @@
       <c r="J14" s="5" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="31.5">
+      <c r="K14" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="31.5">
       <c r="A15" s="4" t="s">
         <v>95</v>
       </c>
@@ -3795,8 +4599,12 @@
       <c r="I15" s="4" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="63">
+      <c r="K15" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" ht="63">
       <c r="A16" s="4" t="s">
         <v>99</v>
       </c>
@@ -3827,8 +4635,14 @@
       <c r="J16" s="5" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75">
+      <c r="K16" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="4" t="s">
         <v>105</v>
       </c>
@@ -3853,8 +4667,12 @@
         <v>548</v>
       </c>
       <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="31.5">
+      <c r="K17" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" ht="31.5">
       <c r="A18" s="4" t="s">
         <v>109</v>
       </c>
@@ -3885,8 +4703,14 @@
       <c r="J18" s="5" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75">
+      <c r="K18" s="5" t="s">
+        <v>706</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="4" t="s">
         <v>115</v>
       </c>
@@ -3908,8 +4732,12 @@
       <c r="I19" s="4" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75">
+      <c r="K19" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="4" t="s">
         <v>119</v>
       </c>
@@ -3931,8 +4759,12 @@
       <c r="I20" s="4" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75">
+      <c r="K20" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="4" t="s">
         <v>124</v>
       </c>
@@ -3960,8 +4792,14 @@
       <c r="J21" s="4" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="315">
+      <c r="K21" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="346.5">
       <c r="A22" s="4" t="s">
         <v>129</v>
       </c>
@@ -3992,8 +4830,14 @@
       <c r="J22" s="5" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="141.75">
+      <c r="K22" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="141.75">
       <c r="A23" s="4" t="s">
         <v>135</v>
       </c>
@@ -4024,8 +4868,14 @@
       <c r="J23" s="5" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="47.25">
+      <c r="K23" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="47.25">
       <c r="A24" s="4" t="s">
         <v>141</v>
       </c>
@@ -4056,8 +4906,14 @@
       <c r="J24" s="5" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75">
+      <c r="K24" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75">
       <c r="A25" s="4" t="s">
         <v>146</v>
       </c>
@@ -4080,8 +4936,12 @@
       <c r="I25" s="4" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="47.25">
+      <c r="K25" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="1:12" ht="47.25">
       <c r="A26" s="4" t="s">
         <v>685</v>
       </c>
@@ -4104,8 +4964,12 @@
       <c r="I26" s="5" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="47.25">
+      <c r="K26" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="1:12" ht="47.25">
       <c r="A27" s="4" t="s">
         <v>154</v>
       </c>
@@ -4136,8 +5000,14 @@
       <c r="J27" s="5" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75">
+      <c r="K27" s="5" t="s">
+        <v>715</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75">
       <c r="A28" s="4" t="s">
         <v>160</v>
       </c>
@@ -4159,6 +5029,10 @@
       <c r="I28" s="4" t="s">
         <v>565</v>
       </c>
+      <c r="K28" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="L28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4173,7 +5047,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4199,27 +5073,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="F6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K6" sqref="F1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="70.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="37.140625" customWidth="1"/>
     <col min="8" max="8" width="86.28515625" customWidth="1"/>
-    <col min="9" max="9" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.140625" customWidth="1"/>
     <col min="10" max="10" width="86.28515625" customWidth="1"/>
+    <col min="11" max="11" width="58.42578125" customWidth="1"/>
+    <col min="12" max="12" width="83.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5">
+    <row r="1" spans="1:12" ht="31.5">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -4232,7 +5108,7 @@
       <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -4241,17 +5117,23 @@
       <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="63">
+      <c r="K1" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="63">
       <c r="A2" s="4" t="s">
         <v>290</v>
       </c>
@@ -4282,8 +5164,14 @@
       <c r="J2" s="5" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="78.75">
+      <c r="K2" t="s">
+        <v>732</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="94.5">
       <c r="A3" s="4" t="s">
         <v>297</v>
       </c>
@@ -4314,8 +5202,14 @@
       <c r="J3" s="5" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="78.75">
+      <c r="K3" t="s">
+        <v>733</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="94.5">
       <c r="A4" s="4" t="s">
         <v>303</v>
       </c>
@@ -4346,8 +5240,14 @@
       <c r="J4" s="5" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="157.5">
+      <c r="K4" t="s">
+        <v>742</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="157.5">
       <c r="A5" s="4" t="s">
         <v>309</v>
       </c>
@@ -4378,8 +5278,14 @@
       <c r="J5" s="5" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="63">
+      <c r="K5" t="s">
+        <v>734</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="63">
       <c r="A6" s="4" t="s">
         <v>315</v>
       </c>
@@ -4410,8 +5316,14 @@
       <c r="J6" s="5" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="110.25">
+      <c r="K6" t="s">
+        <v>735</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="110.25">
       <c r="A7" s="4" t="s">
         <v>321</v>
       </c>
@@ -4442,8 +5354,14 @@
       <c r="J7" s="5" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="78.75">
+      <c r="K7" t="s">
+        <v>736</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="78.75">
       <c r="A8" s="4" t="s">
         <v>327</v>
       </c>
@@ -4474,8 +5392,14 @@
       <c r="J8" s="5" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="110.25">
+      <c r="K8" t="s">
+        <v>737</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="110.25">
       <c r="A9" s="4" t="s">
         <v>332</v>
       </c>
@@ -4506,8 +5430,14 @@
       <c r="J9" s="5" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="63">
+      <c r="K9" t="s">
+        <v>738</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="63">
       <c r="A10" s="4" t="s">
         <v>338</v>
       </c>
@@ -4538,8 +5468,14 @@
       <c r="J10" s="5" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="110.25">
+      <c r="K10" t="s">
+        <v>739</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="110.25">
       <c r="A11" s="4" t="s">
         <v>344</v>
       </c>
@@ -4570,8 +5506,14 @@
       <c r="J11" s="5" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="47.25">
+      <c r="K11" s="17" t="s">
+        <v>740</v>
+      </c>
+      <c r="L11" s="17" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="47.25">
       <c r="A12" s="4" t="s">
         <v>350</v>
       </c>
@@ -4601,6 +5543,12 @@
       </c>
       <c r="J12" s="5" t="s">
         <v>587</v>
+      </c>
+      <c r="K12" t="s">
+        <v>741</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>753</v>
       </c>
     </row>
   </sheetData>
@@ -4618,7 +5566,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4644,10 +5592,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K17" sqref="F1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4662,9 +5610,11 @@
     <col min="8" max="8" width="70.28515625" customWidth="1"/>
     <col min="9" max="9" width="23.7109375" customWidth="1"/>
     <col min="10" max="10" width="70.28515625" customWidth="1"/>
+    <col min="11" max="11" width="71.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="103.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:12" ht="15.75">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -4695,8 +5645,14 @@
       <c r="J1" s="10" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="94.5">
+      <c r="K1" s="10" t="s">
+        <v>687</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="94.5">
       <c r="A2" s="4" t="s">
         <v>165</v>
       </c>
@@ -4727,8 +5683,14 @@
       <c r="J2" s="5" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="63">
+      <c r="K2" t="s">
+        <v>754</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="63">
       <c r="A3" s="4" t="s">
         <v>172</v>
       </c>
@@ -4759,8 +5721,14 @@
       <c r="J3" s="5" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="94.5">
+      <c r="K3" t="s">
+        <v>755</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="94.5">
       <c r="A4" s="4" t="s">
         <v>178</v>
       </c>
@@ -4791,8 +5759,14 @@
       <c r="J4" s="5" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="47.25">
+      <c r="K4" t="s">
+        <v>756</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="47.25">
       <c r="A5" s="4" t="s">
         <v>184</v>
       </c>
@@ -4823,8 +5797,14 @@
       <c r="J5" s="5" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="141.75">
+      <c r="K5" t="s">
+        <v>757</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="141.75">
       <c r="A6" s="4" t="s">
         <v>190</v>
       </c>
@@ -4855,8 +5835,14 @@
       <c r="J6" s="5" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="31.5">
+      <c r="K6" t="s">
+        <v>758</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="31.5">
       <c r="A7" s="4" t="s">
         <v>195</v>
       </c>
@@ -4887,8 +5873,14 @@
       <c r="J7" s="6" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="47.25">
+      <c r="K7" t="s">
+        <v>759</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="47.25">
       <c r="A8" s="4" t="s">
         <v>201</v>
       </c>
@@ -4908,8 +5900,11 @@
       <c r="I8" s="5" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="31.5">
+      <c r="K8" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="31.5">
       <c r="A9" s="4" t="s">
         <v>204</v>
       </c>
@@ -4931,8 +5926,11 @@
       <c r="I9" s="5" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="189">
+      <c r="K9" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="189">
       <c r="A10" s="4" t="s">
         <v>208</v>
       </c>
@@ -4963,8 +5961,14 @@
       <c r="J10" s="5" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="47.25">
+      <c r="K10" t="s">
+        <v>762</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="47.25">
       <c r="A11" s="4" t="s">
         <v>214</v>
       </c>
@@ -4993,8 +5997,14 @@
       <c r="J11" s="5" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="220.5">
+      <c r="K11" t="s">
+        <v>763</v>
+      </c>
+      <c r="L11" s="17" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="220.5">
       <c r="A12" s="4" t="s">
         <v>218</v>
       </c>
@@ -5025,8 +6035,14 @@
       <c r="J12" s="5" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="31.5">
+      <c r="K12" t="s">
+        <v>764</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="31.5">
       <c r="A13" s="4" t="s">
         <v>224</v>
       </c>
@@ -5046,8 +6062,11 @@
       <c r="I13" s="5" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="47.25">
+      <c r="K13" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="47.25">
       <c r="A14" s="4" t="s">
         <v>227</v>
       </c>
@@ -5067,8 +6086,11 @@
       <c r="I14" s="5" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="31.5">
+      <c r="K14" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="31.5">
       <c r="A15" s="4" t="s">
         <v>230</v>
       </c>
@@ -5090,8 +6112,11 @@
       <c r="I15" s="5" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="47.25">
+      <c r="K15" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="47.25">
       <c r="A16" s="4" t="s">
         <v>234</v>
       </c>
@@ -5120,8 +6145,14 @@
         <v>611</v>
       </c>
       <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" ht="31.5">
+      <c r="K16" t="s">
+        <v>768</v>
+      </c>
+      <c r="L16" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="31.5">
       <c r="A17" s="4" t="s">
         <v>240</v>
       </c>
@@ -5143,8 +6174,11 @@
       <c r="I17" s="5" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="47.25">
+      <c r="K17" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="47.25">
       <c r="A18" s="4" t="s">
         <v>244</v>
       </c>
@@ -5164,8 +6198,11 @@
       <c r="I18" s="5" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="110.25">
+      <c r="K18" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="110.25">
       <c r="A19" s="4" t="s">
         <v>247</v>
       </c>
@@ -5196,8 +6233,14 @@
       <c r="J19" s="5" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="47.25">
+      <c r="K19" t="s">
+        <v>771</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="47.25">
       <c r="A20" s="4" t="s">
         <v>252</v>
       </c>
@@ -5217,8 +6260,11 @@
       <c r="I20" s="5" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="110.25">
+      <c r="K20" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="110.25">
       <c r="A21" s="4" t="s">
         <v>255</v>
       </c>
@@ -5249,8 +6295,14 @@
       <c r="J21" s="5" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="47.25">
+      <c r="K21" t="s">
+        <v>773</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="47.25">
       <c r="A22" s="4" t="s">
         <v>261</v>
       </c>
@@ -5281,8 +6333,14 @@
       <c r="J22" s="4" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="47.25">
+      <c r="K22" t="s">
+        <v>774</v>
+      </c>
+      <c r="L22" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="47.25">
       <c r="A23" s="4" t="s">
         <v>267</v>
       </c>
@@ -5313,8 +6371,14 @@
       <c r="J23" s="5" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="110.25">
+      <c r="K23" t="s">
+        <v>775</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="110.25">
       <c r="A24" s="4" t="s">
         <v>272</v>
       </c>
@@ -5345,8 +6409,14 @@
       <c r="J24" s="5" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="47.25">
+      <c r="K24" t="s">
+        <v>776</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="47.25">
       <c r="A25" s="4" t="s">
         <v>278</v>
       </c>
@@ -5377,8 +6447,14 @@
       <c r="J25" s="5" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="47.25">
+      <c r="K25" t="s">
+        <v>777</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="47.25">
       <c r="A26" s="4" t="s">
         <v>284</v>
       </c>
@@ -5409,8 +6485,14 @@
       <c r="J26" s="5" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75">
+      <c r="K26" t="s">
+        <v>778</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75">
       <c r="G27" s="5"/>
       <c r="I27" s="5"/>
     </row>
@@ -5429,7 +6511,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5455,27 +6537,29 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J12" sqref="B1:J1048576"/>
+    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K1" sqref="E1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+    <col min="5" max="5" width="75.140625" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="52.85546875" customWidth="1"/>
     <col min="8" max="8" width="82" customWidth="1"/>
     <col min="9" max="9" width="41.42578125" customWidth="1"/>
     <col min="10" max="10" width="82" customWidth="1"/>
+    <col min="11" max="11" width="53.28515625" customWidth="1"/>
+    <col min="12" max="12" width="83.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5">
+    <row r="1" spans="1:12" ht="15.75">
       <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
@@ -5506,8 +6590,14 @@
       <c r="J1" s="3" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="110.25">
+      <c r="K1" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="110.25">
       <c r="A2" s="12" t="s">
         <v>356</v>
       </c>
@@ -5538,8 +6628,14 @@
       <c r="J2" s="13" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="157.5">
+      <c r="K2" s="18" t="s">
+        <v>796</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="122.25" customHeight="1">
       <c r="A3" s="12" t="s">
         <v>362</v>
       </c>
@@ -5570,8 +6666,14 @@
       <c r="J3" s="13" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="236.25">
+      <c r="K3" s="18" t="s">
+        <v>797</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="141.75">
       <c r="A4" s="12" t="s">
         <v>367</v>
       </c>
@@ -5602,8 +6704,14 @@
       <c r="J4" s="13" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="267.75">
+      <c r="K4" s="18" t="s">
+        <v>798</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="220.5">
       <c r="A5" s="12" t="s">
         <v>373</v>
       </c>
@@ -5634,8 +6742,14 @@
       <c r="J5" s="13" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="362.25">
+      <c r="K5" s="18" t="s">
+        <v>799</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="247.5" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>378</v>
       </c>
@@ -5666,8 +6780,14 @@
       <c r="J6" s="13" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="299.25">
+      <c r="K6" s="19" t="s">
+        <v>800</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="220.5">
       <c r="A7" s="12" t="s">
         <v>382</v>
       </c>
@@ -5698,8 +6818,14 @@
       <c r="J7" s="13" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="393.75">
+      <c r="K7" s="18" t="s">
+        <v>801</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="240">
       <c r="A8" s="12" t="s">
         <v>388</v>
       </c>
@@ -5730,8 +6856,14 @@
       <c r="J8" s="13" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="94.5">
+      <c r="K8" s="12" t="s">
+        <v>817</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="78.75">
       <c r="A9" s="12" t="s">
         <v>394</v>
       </c>
@@ -5762,8 +6894,14 @@
       <c r="J9" s="13" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="31.5">
+      <c r="K9" s="18" t="s">
+        <v>816</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="31.5">
       <c r="A10" s="12" t="s">
         <v>400</v>
       </c>
@@ -5785,8 +6923,11 @@
       <c r="I10" s="12" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="31.5">
+      <c r="K10" s="18" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="31.5">
       <c r="A11" s="12" t="s">
         <v>404</v>
       </c>
@@ -5808,8 +6949,11 @@
       <c r="I11" s="12" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="94.5">
+      <c r="K11" s="18" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="63">
       <c r="A12" s="12" t="s">
         <v>407</v>
       </c>
@@ -5840,8 +6984,14 @@
       <c r="J12" s="13" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="110.25">
+      <c r="K12" t="s">
+        <v>818</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="78.75">
       <c r="A13" s="12" t="s">
         <v>412</v>
       </c>
@@ -5872,8 +7022,14 @@
       <c r="J13" s="13" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="47.25">
+      <c r="K13" t="s">
+        <v>819</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="31.5">
       <c r="A14" s="12" t="s">
         <v>417</v>
       </c>
@@ -5904,8 +7060,14 @@
       <c r="J14" s="13" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75">
+      <c r="K14" s="18" t="s">
+        <v>803</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="12" t="s">
         <v>423</v>
       </c>
@@ -5936,8 +7098,14 @@
       <c r="J15" s="12" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="63">
+      <c r="K15" s="18" t="s">
+        <v>820</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="47.25">
       <c r="A16" s="12" t="s">
         <v>429</v>
       </c>
@@ -5968,8 +7136,14 @@
       <c r="J16" s="13" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75">
+      <c r="K16" s="18" t="s">
+        <v>821</v>
+      </c>
+      <c r="L16" s="17" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="12" t="s">
         <v>436</v>
       </c>
@@ -6000,8 +7174,14 @@
       <c r="J17" s="12" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="63">
+      <c r="K17" s="18" t="s">
+        <v>822</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="47.25">
       <c r="A18" s="12" t="s">
         <v>441</v>
       </c>
@@ -6032,8 +7212,14 @@
       <c r="J18" s="13" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="63">
+      <c r="K18" s="18" t="s">
+        <v>804</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="47.25">
       <c r="A19" s="12" t="s">
         <v>446</v>
       </c>
@@ -6064,8 +7250,14 @@
       <c r="J19" s="13" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="47.25">
+      <c r="K19" s="18" t="s">
+        <v>805</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="31.5">
       <c r="A20" s="12" t="s">
         <v>452</v>
       </c>
@@ -6096,8 +7288,14 @@
       <c r="J20" s="13" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="47.25">
+      <c r="K20" s="18" t="s">
+        <v>806</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="31.5">
       <c r="A21" s="12" t="s">
         <v>458</v>
       </c>
@@ -6128,8 +7326,14 @@
       <c r="J21" s="13" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="47.25">
+      <c r="K21" s="18" t="s">
+        <v>807</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="31.5">
       <c r="A22" s="13" t="s">
         <v>464</v>
       </c>
@@ -6160,8 +7364,14 @@
       <c r="J22" s="13" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="31.5">
+      <c r="K22" s="18" t="s">
+        <v>808</v>
+      </c>
+      <c r="L22" s="17" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75">
       <c r="A23" s="15" t="s">
         <v>469</v>
       </c>
@@ -6192,8 +7402,14 @@
       <c r="J23" s="13" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="31.5">
+      <c r="K23" s="18" t="s">
+        <v>809</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="31.5">
       <c r="A24" s="13" t="s">
         <v>474</v>
       </c>
@@ -6224,8 +7440,14 @@
       <c r="J24" s="13" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="78.75">
+      <c r="K24" s="18" t="s">
+        <v>475</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="63">
       <c r="A25" s="12" t="s">
         <v>478</v>
       </c>
@@ -6256,8 +7478,14 @@
       <c r="J25" s="13" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="110.25">
+      <c r="K25" s="18" t="s">
+        <v>810</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="63">
       <c r="A26" s="13" t="s">
         <v>483</v>
       </c>
@@ -6288,8 +7516,14 @@
       <c r="J26" s="13" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="47.25">
+      <c r="K26" s="18" t="s">
+        <v>811</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="31.5">
       <c r="A27" s="12" t="s">
         <v>489</v>
       </c>
@@ -6320,8 +7554,14 @@
       <c r="J27" s="13" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="47.25">
+      <c r="K27" s="18" t="s">
+        <v>812</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="31.5">
       <c r="A28" s="12" t="s">
         <v>495</v>
       </c>
@@ -6352,8 +7592,14 @@
       <c r="J28" s="13" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="47.25">
+      <c r="K28" s="18" t="s">
+        <v>813</v>
+      </c>
+      <c r="L28" s="17" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="54.75" customHeight="1">
       <c r="A29" s="12" t="s">
         <v>500</v>
       </c>
@@ -6384,8 +7630,14 @@
       <c r="J29" s="13" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="63">
+      <c r="K29" s="18" t="s">
+        <v>814</v>
+      </c>
+      <c r="L29" s="17" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="47.25">
       <c r="A30" s="13" t="s">
         <v>506</v>
       </c>
@@ -6416,8 +7668,14 @@
       <c r="J30" s="13" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="63">
+      <c r="K30" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="L30" s="17" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="47.25">
       <c r="A31" s="12" t="s">
         <v>511</v>
       </c>
@@ -6448,8 +7706,14 @@
       <c r="J31" s="13" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="94.5">
+      <c r="K31" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="63">
       <c r="A32" s="12" t="s">
         <v>515</v>
       </c>
@@ -6479,6 +7743,12 @@
       </c>
       <c r="J32" s="13" t="s">
         <v>682</v>
+      </c>
+      <c r="K32" s="18" t="s">
+        <v>815</v>
+      </c>
+      <c r="L32" s="17" t="s">
+        <v>848</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(lib): add Spanish translation to doc-pol library (#3150)
Replace doc-pol_new.xlsx with Spanish version
</commit_message>
<xml_diff>
--- a/tools/excel/intuitem/doc-pol_new.xlsx
+++ b/tools/excel/intuitem/doc-pol_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ciso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thidalgo.INDRA\OneDrive - Indra\Documentos\CISO_ASSISTANT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B9D3A5-D92B-4699-B0E0-179179FCBE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAEFAC6-EA65-4123-B562-35BECC95C9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="747" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="854">
   <si>
     <t>type</t>
   </si>
@@ -2762,6 +2762,709 @@
 Retention rules
 Use of test information
 Continual improvement</t>
+  </si>
+  <si>
+    <t>name[es]</t>
+  </si>
+  <si>
+    <t>description[es]</t>
+  </si>
+  <si>
+    <t>Documentación, políticas, procedimientos, formación y controles técnicos habituales recomendados por Intuitem</t>
+  </si>
+  <si>
+    <t>Documento de visión general de la organización</t>
+  </si>
+  <si>
+    <t>Documento de contexto de la organización</t>
+  </si>
+  <si>
+    <t>Documento de alcance del SGSI</t>
+  </si>
+  <si>
+    <t>Registro legal</t>
+  </si>
+  <si>
+    <t>Documento de declaración de aplicabilidad</t>
+  </si>
+  <si>
+    <t>Matriz de responsabilidad de los controles</t>
+  </si>
+  <si>
+    <t>Documento del plan de auditoría</t>
+  </si>
+  <si>
+    <t>Matriz de competencias</t>
+  </si>
+  <si>
+    <t>Matriz de responsabilidades</t>
+  </si>
+  <si>
+    <t>Documento del plan de comunicación</t>
+  </si>
+  <si>
+    <t>Registro de riesgos</t>
+  </si>
+  <si>
+    <t>Registro de objetivos de seguridad</t>
+  </si>
+  <si>
+    <t>Documento del plan de revisión por la dirección</t>
+  </si>
+  <si>
+    <t>Registro de formación y concienciación</t>
+  </si>
+  <si>
+    <t>Registro de documentos</t>
+  </si>
+  <si>
+    <t>Registro de procedimientos operativos</t>
+  </si>
+  <si>
+    <t>Registro de no conformidades</t>
+  </si>
+  <si>
+    <t>Documento de normas de funcionamiento</t>
+  </si>
+  <si>
+    <t>Registro de activos</t>
+  </si>
+  <si>
+    <t>Registro de proveedores</t>
+  </si>
+  <si>
+    <t>Plan de concienciación y formación en seguridad de la información</t>
+  </si>
+  <si>
+    <t>Plan de aseguramiento de la seguridad</t>
+  </si>
+  <si>
+    <t>Mapa del sistema de información</t>
+  </si>
+  <si>
+    <t>Registro de cuentas de acceso privilegiado</t>
+  </si>
+  <si>
+    <t>Registro de incidentes de seguridad</t>
+  </si>
+  <si>
+    <t>Matriz de flujos</t>
+  </si>
+  <si>
+    <t>Principios de arquitectura de seguridad</t>
+  </si>
+  <si>
+    <t>Objetivos de la organización
+Organigrama
+Objetivos del SGSI
+Responsabilidades del CISO
+Revisión del SGSI por la dirección</t>
+  </si>
+  <si>
+    <t>Partes interesadas
+Autoridades
+Grupos de interés especial</t>
+  </si>
+  <si>
+    <t>Productos y servicios
+Productos y servicios que requieren certificación
+Ubicaciones
+Vista de la organización
+Vista de la arquitectura de negocio
+Vista de la arquitectura de datos
+Vista de la arquitectura de aplicaciones
+Vista de la arquitectura tecnológica
+Vista de la red
+Declaración de alcance</t>
+  </si>
+  <si>
+    <t>Requisitos legales
+Requisitos estatutarios
+Requisitos reglamentarios
+Requisitos contractuales
+Derechos de propiedad intelectual
+Contratos laborales
+Acuerdos de confidencialidad</t>
+  </si>
+  <si>
+    <t>Contexto de la organización
+Liderazgo
+Planificación
+Soporte
+Operación
+Evaluación del desempeño
+Mejora
+Controles organizativos
+Controles de las personas
+Controles físicos
+Controles tecnológicos</t>
+  </si>
+  <si>
+    <t>RACI para el SGSI</t>
+  </si>
+  <si>
+    <t>Propietario del riesgo
+Impacto
+Probabilidad
+Nivel de riesgo
+Evaluación
+Prioridad
+Opción de tratamiento
+Mitigaciones – medidas de seguridad recomendadas</t>
+  </si>
+  <si>
+    <t>Revisión de riesgos
+Revisión de los objetivos de seguridad
+Revisión de los incidentes de seguridad
+Revisión de la gestión de vulnerabilidades
+Revisión de las no conformidades</t>
+  </si>
+  <si>
+    <t>Normas para la edición y el mantenimiento
+Control de versiones
+Registro
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Lista de no conformidades (incidentes, problemas, …)
+Acción correctiva adoptada</t>
+  </si>
+  <si>
+    <t>Gestión de riesgos</t>
+  </si>
+  <si>
+    <t>Objetivo: Sensibilizar a todos los empleados y proporcionar formación específica al personal pertinente para promover comportamientos seguros, garantizar el cumplimiento y reducir los riesgos.
+Alcance: Concienciación para todos los empleados y contratistas; formación específica para determinados equipos (por ejemplo, TI, seguridad, gestores de accesos).
+Funciones y responsabilidades: Asignar responsabilidades a los equipos de TI, RR. HH. y seguridad.
+Requisitos de formación: Definir los contenidos obligatorios (por ejemplo, gestión de accesos, configuraciones seguras) y la periodicidad (por ejemplo, anual, incorporación).
+Métodos de impartición: Concienciación mediante formación en línea y campañas; formación mediante talleres prácticos y simulaciones.
+Evaluación: Realizar el seguimiento de las tasas de participación, los resultados de los cuestionarios y los resultados de las pruebas de phishing.
+Cumplimiento: Alinear con la normativa (por ejemplo, RGPD, ISO 27001) y mantener registros preparados para auditoría.
+Mejora continua: Actualizar en función de la retroalimentación y de las amenazas emergentes.</t>
+  </si>
+  <si>
+    <t>Documento proporcionado por los proveedores que describe las medidas de seguridad, el cumplimiento de normas (por ejemplo, ISO 27001) y los procedimientos de prueba para garantizar la seguridad de sus productos, servicios o sistemas. Demuestra su compromiso con el mantenimiento de un entorno seguro y proporciona evidencias de cumplimiento y de las prácticas de seguridad.</t>
+  </si>
+  <si>
+    <t>Representación visual de los componentes del sistema de información de una organización y de sus interacciones para mejorar su gestión y seguridad.</t>
+  </si>
+  <si>
+    <t>Documento que mapea los flujos de datos autorizados entre sistemas, aplicaciones o zonas de red para garantizar una comunicación segura y conforme a los requisitos.</t>
+  </si>
+  <si>
+    <t>Procedimiento de gestión de accesos privilegiados</t>
+  </si>
+  <si>
+    <t>Procedimiento de recertificación de cuentas</t>
+  </si>
+  <si>
+    <t>Procedimiento de seguridad física</t>
+  </si>
+  <si>
+    <t>Procedimiento de objetos de directiva de grupo</t>
+  </si>
+  <si>
+    <t>Procedimiento de gestión de actualizaciones</t>
+  </si>
+  <si>
+    <t>Procedimiento de gestión de incidentes</t>
+  </si>
+  <si>
+    <t>Procedimiento de eliminación segura</t>
+  </si>
+  <si>
+    <t>Procedimiento de sincronización horaria</t>
+  </si>
+  <si>
+    <t>Procedimiento de configuración de la seguridad del correo electrónico</t>
+  </si>
+  <si>
+    <t>Procedimiento de registro de eventos</t>
+  </si>
+  <si>
+    <t>Procedimiento de seguridad de RR.HH.</t>
+  </si>
+  <si>
+    <t>Documento que describe los procesos y controles para la gestión y protección de las cuentas privilegiadas, garantizando que únicamente los usuarios autorizados tengan acceso a los sistemas y datos críticos, mediante medidas como la monitorización, la auditoría y el acceso con tiempo limitado para minimizar los riesgos.</t>
+  </si>
+  <si>
+    <t>Documento que define el proceso para la revisión y validación periódicas de los derechos de acceso de los usuarios, las certificaciones de los sistemas o el cumplimiento de normas. Garantiza que solo los usuarios y sistemas autorizados mantengan el acceso o la certificación, y ayuda a identificar y revocar permisos obsoletos o innecesarios.</t>
+  </si>
+  <si>
+    <t>Documento que describe los procesos y controles relacionados con la gestión de los recursos humanos dentro de una organización, garantizando el cumplimiento de los requisitos legales, reglamentarios y de seguridad. Incluye los procedimientos de selección, incorporación, cambios de puesto, formación y finalización de la relación laboral para proteger la información y los activos de la organización.</t>
+  </si>
+  <si>
+    <t>Documento que define cómo crear, configurar y gestionar los GPO para aplicar ajustes de seguridad, configuraciones del sistema y políticas de usuario en un entorno Windows. Garantiza la aplicación coherente de las políticas organizativas para unas operaciones de TI seguras y conformes.</t>
+  </si>
+  <si>
+    <t>Control de accesos: Procedimientos para conceder, revocar y supervisar el acceso físico a las áreas seguras.
+Protección de activos: Directrices para la protección de los activos críticos (por ejemplo, servidores, dispositivos de almacenamiento).
+Vigilancia: Uso de cámaras, alarmas y sistemas de monitorización para detectar y prevenir intrusiones.
+Gestión de visitantes: Políticas para el registro y el acompañamiento de visitantes en áreas seguras.
+Respuesta ante incidentes: Pasos para abordar brechas de seguridad física o situaciones de emergencia.</t>
+  </si>
+  <si>
+    <t>Funciones y responsabilidades
+Clasificación de las actualizaciones
+Planificación de las actualizaciones
+Pruebas y validación
+Proceso de despliegue
+Supervisión y verificación
+Documentación y elaboración de informes</t>
+  </si>
+  <si>
+    <t>Implementación práctica de la política de gestión de incidentes</t>
+  </si>
+  <si>
+    <t>Funciones y responsabilidades
+Identificación de activos para su eliminación
+Métodos de eliminación segura
+Saneado de datos
+Cumplimiento de los requisitos legales y reglamentarios
+Documentación y mantenimiento de registros
+Verificación y auditoría</t>
+  </si>
+  <si>
+    <t>Fuente horaria: Uso de fuentes externas fiables (por ejemplo, servidores NTP).
+Configuración: Definición de intervalos de sincronización y mecanismos de respaldo.
+Supervisión: Verificación periódica del estado de la sincronización horaria.</t>
+  </si>
+  <si>
+    <t>Configuración del servidor de correo electrónico
+Protección del correo electrónico basada en dominios
+Controles antimalware y antispam
+Cifrado y comunicaciones seguras
+Control de accesos y monitorización
+Copia de seguridad y recuperación
+Concienciación y formación de los usuarios</t>
+  </si>
+  <si>
+    <t>Recogida y categorización de registros
+Políticas de almacenamiento seguro y conservación
+Análisis para la detección de anomalías y la respuesta a incidentes</t>
+  </si>
+  <si>
+    <t>Política principal</t>
+  </si>
+  <si>
+    <t>Política de concienciación y formación en seguridad de la información</t>
+  </si>
+  <si>
+    <t>Política de puestos de trabajo y teletrabajo</t>
+  </si>
+  <si>
+    <t>Política criptográfica</t>
+  </si>
+  <si>
+    <t>Política de clasificación y tratamiento de la información</t>
+  </si>
+  <si>
+    <t>Política de auditoría interna y externa</t>
+  </si>
+  <si>
+    <t>Política de continuidad de negocio</t>
+  </si>
+  <si>
+    <t>Política de segregación de funciones</t>
+  </si>
+  <si>
+    <t>Política de control de accesos</t>
+  </si>
+  <si>
+    <t>Política de protección frente a malware</t>
+  </si>
+  <si>
+    <t>Política de gestión de riesgos</t>
+  </si>
+  <si>
+    <t>Política de gestión de activos</t>
+  </si>
+  <si>
+    <t>Política de copia de seguridad y restauración</t>
+  </si>
+  <si>
+    <t>Política de seguridad de proveedores externos</t>
+  </si>
+  <si>
+    <t>Política de registro y monitorización</t>
+  </si>
+  <si>
+    <t>Política de transferencia de la información</t>
+  </si>
+  <si>
+    <t>Política de desarrollo seguro</t>
+  </si>
+  <si>
+    <t>Política de seguridad física</t>
+  </si>
+  <si>
+    <t>Política de gestión de la seguridad de red</t>
+  </si>
+  <si>
+    <t>Política de uso aceptable</t>
+  </si>
+  <si>
+    <t>Política de integración de proyectos de sistemas de información</t>
+  </si>
+  <si>
+    <t>Política de inteligencia de amenazas</t>
+  </si>
+  <si>
+    <t>Política de gestión de incidentes de seguridad de la información</t>
+  </si>
+  <si>
+    <t>Política de mantenimiento</t>
+  </si>
+  <si>
+    <t>Política de gestión de vulnerabilidades</t>
+  </si>
+  <si>
+    <t>Objetivos de seguridad de la información
+Compromiso
+Revisión por la dirección
+Políticas aplicables
+Gestión de las no conformidades
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Implicaciones del incumplimiento
+Notificación de eventos de seguridad
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Puestos de trabajo
+Dispositivos móviles
+Teletrabajo
+Gestión de contraseñas
+Devolución de activos
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Gestión de claves
+Cifrado
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Clasificación
+Protección y tratamiento de la información
+Protección y tratamiento de los datos personales
+Mesa limpia
+Pantalla limpia
+Protección de los registros
+Normas de conservación
+Uso de información de prueba
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Protección de la información de auditoría</t>
+  </si>
+  <si>
+    <t>Identificación
+Autenticación
+Gestión de contraseñas
+RBAC (control de acceso basado en roles)
+Revisión de los derechos de acceso
+Aprovisionamiento
+Bajas de usuarios
+Acceso remoto
+Gestión de accesos privilegiados
+Acceso de terceros
+Supervisión y elaboración de informes
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Antivirus
+EDR</t>
+  </si>
+  <si>
+    <t>Definición de la gestión de riesgos
+Apetito de riesgo
+Criterios de aceptación del riesgo
+Criterios para la evaluación de riesgos
+Identificación de riesgos
+Evaluación de riesgos
+Enfoque CIAP
+Informes de riesgos
+Revisión de riesgos
+Tratamiento del riesgo (mitigación, aceptación, transferencia)
+Evaluación del riesgo
+Uso de los controles de la ISO/IEC 27002
+Gestión de los derechos de acceso
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Registro de eventos</t>
+  </si>
+  <si>
+    <t>Perímetro de seguridad física
+Áreas seguras
+Control de acceso de empleados
+Control de acceso de visitantes
+Gestión de entregas
+Seguridad del cableado
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Objetivo: Definir los usos permitidos y prohibidos de los recursos.
+Alcance: Todos los usuarios de los sistemas de información.
+Normas: Actividades permitidas y prohibidas, obligaciones de seguridad.
+Confidencialidad: Protección de los datos sensibles.
+Cumplimiento: Supervisión y sanciones por incumplimiento.</t>
+  </si>
+  <si>
+    <t>Normas para la integración de la seguridad en los proyectos de sistemas de información</t>
+  </si>
+  <si>
+    <t>Vulnerabilidades conocidas explotadas
+Actividad de actores de amenazas
+Mejora continua</t>
+  </si>
+  <si>
+    <t>Clasificación de incidentes
+Notificación de incidentes
+Proceso de respuesta a incidentes
+Análisis de la causa raíz y lecciones aprendidas
+Documentación y comunicación
+Funciones y responsabilidades
+Revisión y actualización</t>
+  </si>
+  <si>
+    <t>Gestión de la obsolescencia
+Contratos de mantenimiento
+Gestión de cambios</t>
+  </si>
+  <si>
+    <t>Detección y gestión de vulnerabilidades
+Gestión de parches</t>
+  </si>
+  <si>
+    <t>Formación en requisitos legales y reglamentarios</t>
+  </si>
+  <si>
+    <t>Formación sobre el panorama de amenazas</t>
+  </si>
+  <si>
+    <t>Formación en IAM (gestión de identidades y accesos)</t>
+  </si>
+  <si>
+    <t>Formación en seguridad de red</t>
+  </si>
+  <si>
+    <t>Formación en mantenimiento de condiciones de seguridad (SCM)</t>
+  </si>
+  <si>
+    <t>Formación en registro y monitorización</t>
+  </si>
+  <si>
+    <t>Registro de accesos</t>
+  </si>
+  <si>
+    <t>Antivirus de host, cortafuegos y control de USB</t>
+  </si>
+  <si>
+    <t>Base de datos de gestión de la configuración (CMDB)</t>
+  </si>
+  <si>
+    <t>Gestión de información y eventos de seguridad (SIEM)</t>
+  </si>
+  <si>
+    <t>Filtro de pantalla</t>
+  </si>
+  <si>
+    <t>Cortafuegos de red</t>
+  </si>
+  <si>
+    <t>Pasarela de correo seguro</t>
+  </si>
+  <si>
+    <t>Antivirus de red</t>
+  </si>
+  <si>
+    <t>Microsegmentación</t>
+  </si>
+  <si>
+    <t>Seguridad Wi-Fi</t>
+  </si>
+  <si>
+    <t>Proxy inverso</t>
+  </si>
+  <si>
+    <t>Cortafuegos de aplicaciones web (WAF)</t>
+  </si>
+  <si>
+    <t>Sistema de detección de intrusiones (IDS)</t>
+  </si>
+  <si>
+    <t>Autenticación multifactor (MFA)</t>
+  </si>
+  <si>
+    <t>Control de acceso a la red (NAC)(802.1X)</t>
+  </si>
+  <si>
+    <t>Formación en bastionado y configuración segura</t>
+  </si>
+  <si>
+    <t>Gestión de contraseñas</t>
+  </si>
+  <si>
+    <t>Gestión unificada de endpoints</t>
+  </si>
+  <si>
+    <t>Cifrado de discos</t>
+  </si>
+  <si>
+    <t>Copias de seguridad inmutables</t>
+  </si>
+  <si>
+    <t>Cifrado de archivos</t>
+  </si>
+  <si>
+    <t>Detección y respuesta de eventos (EDR)</t>
+  </si>
+  <si>
+    <t>Objetivo: Garantizar la concienciación sobre el cumplimiento de los requisitos legales y reglamentarios.
+Destinatarios: Todos los empleados; adaptado a funciones específicas.
+Contenidos: Principales normativas (por ejemplo, RGPD), tratamiento de datos, riesgos del incumplimiento.
+Métodos: Formación en línea, talleres y estudios de casos.
+Evaluación: Cuestionarios y pruebas basadas en escenarios.</t>
+  </si>
+  <si>
+    <t>Objetivo: Comprender las amenazas cibernéticas actuales y las estrategias de mitigación.
+Destinatarios: Personal de TI, equipos de seguridad y responsables de la toma de decisiones.
+Contenidos: Amenazas emergentes, técnicas de ataque y mecanismos de defensa.
+Métodos: Presentaciones, estudios de casos y debates basados en escenarios.
+Resultado: Mayor concienciación y preparación para hacer frente a amenazas en evolución.</t>
+  </si>
+  <si>
+    <t>Objetivo: Comprender y dominar la gestión de identidades y accesos.
+Destinatarios: Administradores de TI, equipos de seguridad y gestores de accesos.
+Contenidos:
+-Conceptos clave (identidad, autenticación, autorización, modelos RBAC/ABAC).
+-Buenas prácticas de IAM (gestión de derechos, aprovisionamiento, auditorías).
+-Normas y herramientas (SAML, OAuth, Active Directory, etc.).
+Métodos: Talleres prácticos, casos de uso y demostraciones.
+Resultado: Mejora de las capacidades para proteger y gestionar los accesos de forma segura y eficiente.</t>
+  </si>
+  <si>
+    <t>Objetivo: Desarrollar la especialización en el mantenimiento de sistemas de TI seguros mediante la monitorización, la gestión de parches, el cumplimiento y la respuesta a incidentes.
+Destinatarios: Profesionales de seguridad de TI, administradores de sistemas, responsables de cumplimiento y equipos de respuesta a incidentes.
+Contenidos:
+-Principios del mantenimiento de la seguridad y su importancia en la ciberseguridad.
+-Herramientas y técnicas de monitorización de la seguridad (por ejemplo, SIEM, IDS).
+-Gestión de parches y configuraciones seguras de los sistemas.
+-Detección de incidentes, planificación de la respuesta y ejecución.
+-Cumplimiento de las políticas de seguridad y de los requisitos normativos.
+Métodos: Laboratorios prácticos, escenarios simulados y estudios de casos sobre el mantenimiento de las condiciones de seguridad.
+Resultado: Mejora de la capacidad para proteger de forma continua los entornos de TI, mitigar riesgos y garantizar el cumplimiento.</t>
+  </si>
+  <si>
+    <t>Objetivo: Enseñar prácticas eficaces de registro de eventos y técnicas de monitorización para reforzar la seguridad y la respuesta a incidentes.
+Destinatarios: Administradores de TI, equipos de seguridad y analistas de SOC.
+Contenidos:
+-Importancia del registro de eventos y de los requisitos de cumplimiento.
+-Configuración y gestión de las fuentes de registro (por ejemplo, servidores, cortafuegos, aplicaciones).
+-Sistemas centralizados de registro de eventos (por ejemplo, SIEM, pila ELK).
+-Detección de anomalías y análisis de registros.
+-Respuesta a incidentes basada en la información obtenida de los registros.
+Métodos: Laboratorios prácticos, escenarios reales y ejercicios de análisis de registros.
+Resultado: Mejora de la capacidad para recopilar, analizar y actuar sobre los datos de registro con el fin de prevenir y responder a incidentes.</t>
+  </si>
+  <si>
+    <t>Objetivo: Dotar a los participantes de los conocimientos necesarios para implementar configuraciones seguras y bastionar los sistemas con el fin de reducir vulnerabilidades.
+Destinatarios: Administradores de TI, ingenieros de sistemas y profesionales de la seguridad.
+Contenidos:
+-Principios del bastionado de sistemas.
+-Bastionado de sistemas operativos (Windows, Linux).
+-Aseguramiento de bases de datos (por ejemplo, MySQL, PostgreSQL).
+-Bastionado de dispositivos de red (cortafuegos, routers, switches).
+-Aplicación de los CIS Benchmarks y de las directrices de la ANSSI.
+-Herramientas de automatización (por ejemplo, Ansible, Puppet, Chef).
+Métodos:
+-Laboratorios prácticos para el bastionado de sistemas operativos y aplicaciones.
+-Estudios de casos sobre fallos de bastionado y soluciones.
+Resultado: Los participantes adquirirán la capacidad de implementar configuraciones seguras y mejorar la resiliencia global de los sistemas.</t>
+  </si>
+  <si>
+    <t>Mecanismo que aplica a la autenticación y la autorización de dispositivos o usuarios antes de conceder el acceso a la red. Garantiza un acceso seguro a redes cableadas e inalámbricas mediante el uso de protocolos como 802.1X y RADIUS para validar credenciales y aplicar políticas de acceso.</t>
+  </si>
+  <si>
+    <t>Soluciones integradas para la protección de los endpoints, que incluyen antivirus, cortafuegos y control de puertos USB.</t>
+  </si>
+  <si>
+    <t>Cifrado completo de disco para puestos de trabajo.</t>
+  </si>
+  <si>
+    <t>Utilidades de cifrado de archivos como 7zip.</t>
+  </si>
+  <si>
+    <t>Repositorio centralizado que almacena y gestiona información sobre los activos de TI, sus configuraciones y sus relaciones, para apoyar una gestión eficaz de los sistemas de información.</t>
+  </si>
+  <si>
+    <t>Sistema que recopila, analiza y correlaciona datos de seguridad procedentes de múltiples fuentes para detectar y responder a amenazas.</t>
+  </si>
+  <si>
+    <t>Filtro físico o digital que limita la visibilidad de la pantalla a usuarios autorizados, reduciendo el riesgo de brechas de seguridad por observación visual.</t>
+  </si>
+  <si>
+    <t>Sistema de seguridad que supervisa y controla el tráfico de red entrante y saliente en función de reglas predefinidas.</t>
+  </si>
+  <si>
+    <t>Sistema que filtra, supervisa y protege las comunicaciones de correo electrónico frente a spam, malware y accesos no autorizados.</t>
+  </si>
+  <si>
+    <t>Protege el tráfico de correo electrónico y web en el perímetro de red frente a malware.</t>
+  </si>
+  <si>
+    <t>Las VLAN aíslan y segmentan el tráfico de red para reforzar la seguridad y optimizar el rendimiento.</t>
+  </si>
+  <si>
+    <t>La microsegmentación es una estrategia de seguridad que crea políticas granulares y contextuales para aislar cargas de trabajo o aplicaciones individuales dentro de una red, limitando el movimiento lateral y conteniendo las brechas de seguridad.</t>
+  </si>
+  <si>
+    <t>La seguridad Wi-Fi garantiza comunicaciones inalámbricas seguras mediante cifrado WPA3 Enterprise, autenticación robusta y mecanismos avanzados de control de acceso. Aunque WPA2 Enterprise sigue siendo aceptable, se recomienda encarecidamente la transición a WPA3 para una mayor seguridad.</t>
+  </si>
+  <si>
+    <t>Un proxy inverso reenvía las solicitudes de los clientes a los servidores backend, mejorando la seguridad, el equilibrio de carga y el rendimiento.</t>
+  </si>
+  <si>
+    <t>Un cortafuegos de aplicaciones web (WAF) protege las aplicaciones web filtrando y supervisando el tráfico HTTP para bloquear actividades maliciosas.</t>
+  </si>
+  <si>
+    <t>Un sistema de detección de intrusiones (IDS) supervisa el tráfico de red para detectar y alertar sobre posibles amenazas de seguridad o actividades no autorizadas.</t>
+  </si>
+  <si>
+    <t>Un proxy web filtra y supervisa el tráfico web, aplica políticas de seguridad y permite la autenticación de usuarios para controlar y proteger el acceso a Internet.</t>
+  </si>
+  <si>
+    <t>Una red privada virtual (VPN) protege la transmisión de datos mediante el cifrado del tráfico utilizando protocolos como IPsec, garantizando la confidencialidad y la protección frente a interceptaciones.</t>
+  </si>
+  <si>
+    <t>La autenticación multifactor (MFA) refuerza la seguridad al requerir dos factores de verificación de categorías diferentes: algo que sabes (por ejemplo, una contraseña), algo que tienes (por ejemplo, un token o un teléfono móvil) y algo que eres (por ejemplo, una huella dactilar o reconocimiento facial).</t>
+  </si>
+  <si>
+    <t>Capacidad que permite la creación, el almacenamiento, la gestión y el uso seguros de contraseñas para sistemas, aplicaciones y cuentas. Reduce el riesgo de accesos no autorizados mediante la aplicación de políticas de contraseñas robustas y garantizando un tratamiento seguro de las credenciales.</t>
+  </si>
+  <si>
+    <t>Capacidad que proporciona el control y la gestión centralizados de todos los endpoints, incluidos equipos de sobremesa, portátiles, dispositivos móviles y dispositivos IoT, a través de una única plataforma. Garantiza una configuración segura, la aplicación de políticas, la gestión de aplicaciones y la monitorización en todo el ecosistema de endpoints de la organización.</t>
+  </si>
+  <si>
+    <t>Capacidad que garantiza que las copias de seguridad no puedan ser modificadas, eliminadas ni sobrescritas, protegiendo la integridad de los datos frente a ransomware y accesos no autorizados.</t>
+  </si>
+  <si>
+    <t>Objetivo: Enseñar las mejores prácticas para asegurar las infraestructuras de red y prevenir amenazas cibernéticas.
+Destinatarios: Administradores de TI, ingenieros de redes y profesionales de la seguridad.
+Contenidos:
+-Principios de segregación de redes.
+-Configuración y supervisión de cortafuegos.
+-Sistemas de detección y prevención de intrusiones (IDS/IPS/NDR).
+-Segmentación de red y control de accesos.
+-Protocolos seguros (por ejemplo, HTTPS, VPN, SSH).
+-Mitigación de amenazas (por ejemplo, DDoS, malware).
+  Métodos: Laboratorios interactivos, simulaciones y ejercicios prácticos.
+  Resultado: Mejora de la capacidad para proteger y supervisar entornos de red.</t>
+  </si>
+  <si>
+    <t>Controles de referencia de uso común</t>
   </si>
 </sst>
 </file>
@@ -2846,7 +3549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2888,9 +3591,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3190,16 +3902,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView zoomScale="180" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="76.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="111.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3223,7 +3935,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3312,6 +4024,22 @@
       </c>
       <c r="B14" t="s">
         <v>524</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>687</v>
+      </c>
+      <c r="B15" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>688</v>
+      </c>
+      <c r="B16" t="s">
+        <v>689</v>
       </c>
     </row>
   </sheetData>
@@ -3329,8 +4057,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3356,17 +4084,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K1" sqref="F1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="70.28515625" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
@@ -3374,9 +4102,11 @@
     <col min="8" max="8" width="73.140625" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
     <col min="10" max="10" width="73.140625" customWidth="1"/>
+    <col min="11" max="11" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5">
+    <row r="1" spans="1:12" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -3389,7 +4119,7 @@
       <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -3398,17 +4128,23 @@
       <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="78.75">
+      <c r="K1" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="78.75">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -3439,8 +4175,14 @@
       <c r="J2" s="5" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="63">
+      <c r="K2" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="63">
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
@@ -3471,8 +4213,14 @@
       <c r="J3" s="5" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="157.5">
+      <c r="K3" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="157.5">
       <c r="A4" s="4" t="s">
         <v>41</v>
       </c>
@@ -3503,8 +4251,14 @@
       <c r="J4" s="5" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="110.25">
+      <c r="K4" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="110.25">
       <c r="A5" s="4" t="s">
         <v>47</v>
       </c>
@@ -3535,8 +4289,14 @@
       <c r="J5" s="5" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75">
+      <c r="K5" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -3555,8 +4315,12 @@
       <c r="I6" s="4" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75">
+      <c r="K6" s="5" t="s">
+        <v>694</v>
+      </c>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75">
       <c r="A7" s="4" t="s">
         <v>56</v>
       </c>
@@ -3578,8 +4342,12 @@
       <c r="I7" s="4" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="173.25">
+      <c r="K7" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" ht="173.25">
       <c r="A8" s="4" t="s">
         <v>60</v>
       </c>
@@ -3610,8 +4378,14 @@
       <c r="J8" s="5" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75">
+      <c r="K8" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75">
       <c r="A9" s="4" t="s">
         <v>66</v>
       </c>
@@ -3633,8 +4407,12 @@
       <c r="I9" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75">
+      <c r="K9" s="5" t="s">
+        <v>697</v>
+      </c>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="4" t="s">
         <v>70</v>
       </c>
@@ -3662,8 +4440,14 @@
       <c r="J10" s="4" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75">
+      <c r="K10" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="4" t="s">
         <v>75</v>
       </c>
@@ -3685,8 +4469,12 @@
       <c r="I11" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="141.75">
+      <c r="K11" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" ht="141.75">
       <c r="A12" s="4" t="s">
         <v>79</v>
       </c>
@@ -3717,8 +4505,14 @@
       <c r="J12" s="5" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75">
+      <c r="K12" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75">
       <c r="A13" s="4" t="s">
         <v>85</v>
       </c>
@@ -3740,8 +4534,12 @@
       <c r="I13" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="78.75">
+      <c r="K13" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" ht="78.75">
       <c r="A14" s="4" t="s">
         <v>89</v>
       </c>
@@ -3772,8 +4570,14 @@
       <c r="J14" s="5" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="31.5">
+      <c r="K14" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="31.5">
       <c r="A15" s="4" t="s">
         <v>95</v>
       </c>
@@ -3795,8 +4599,12 @@
       <c r="I15" s="4" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="63">
+      <c r="K15" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" ht="63">
       <c r="A16" s="4" t="s">
         <v>99</v>
       </c>
@@ -3827,8 +4635,14 @@
       <c r="J16" s="5" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75">
+      <c r="K16" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="4" t="s">
         <v>105</v>
       </c>
@@ -3853,8 +4667,12 @@
         <v>548</v>
       </c>
       <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="31.5">
+      <c r="K17" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" ht="31.5">
       <c r="A18" s="4" t="s">
         <v>109</v>
       </c>
@@ -3885,8 +4703,14 @@
       <c r="J18" s="5" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75">
+      <c r="K18" s="5" t="s">
+        <v>706</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="4" t="s">
         <v>115</v>
       </c>
@@ -3908,8 +4732,12 @@
       <c r="I19" s="4" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75">
+      <c r="K19" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="4" t="s">
         <v>119</v>
       </c>
@@ -3931,8 +4759,12 @@
       <c r="I20" s="4" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75">
+      <c r="K20" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="4" t="s">
         <v>124</v>
       </c>
@@ -3960,8 +4792,14 @@
       <c r="J21" s="4" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="315">
+      <c r="K21" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="346.5">
       <c r="A22" s="4" t="s">
         <v>129</v>
       </c>
@@ -3992,8 +4830,14 @@
       <c r="J22" s="5" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="141.75">
+      <c r="K22" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="141.75">
       <c r="A23" s="4" t="s">
         <v>135</v>
       </c>
@@ -4024,8 +4868,14 @@
       <c r="J23" s="5" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="47.25">
+      <c r="K23" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="47.25">
       <c r="A24" s="4" t="s">
         <v>141</v>
       </c>
@@ -4056,8 +4906,14 @@
       <c r="J24" s="5" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75">
+      <c r="K24" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75">
       <c r="A25" s="4" t="s">
         <v>146</v>
       </c>
@@ -4080,8 +4936,12 @@
       <c r="I25" s="4" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="47.25">
+      <c r="K25" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="1:12" ht="47.25">
       <c r="A26" s="4" t="s">
         <v>685</v>
       </c>
@@ -4104,8 +4964,12 @@
       <c r="I26" s="5" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="47.25">
+      <c r="K26" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="1:12" ht="47.25">
       <c r="A27" s="4" t="s">
         <v>154</v>
       </c>
@@ -4136,8 +5000,14 @@
       <c r="J27" s="5" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75">
+      <c r="K27" s="5" t="s">
+        <v>715</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75">
       <c r="A28" s="4" t="s">
         <v>160</v>
       </c>
@@ -4159,6 +5029,10 @@
       <c r="I28" s="4" t="s">
         <v>565</v>
       </c>
+      <c r="K28" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="L28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4173,7 +5047,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4199,27 +5073,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="F6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K6" sqref="F1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="70.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="37.140625" customWidth="1"/>
     <col min="8" max="8" width="86.28515625" customWidth="1"/>
-    <col min="9" max="9" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.140625" customWidth="1"/>
     <col min="10" max="10" width="86.28515625" customWidth="1"/>
+    <col min="11" max="11" width="58.42578125" customWidth="1"/>
+    <col min="12" max="12" width="83.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5">
+    <row r="1" spans="1:12" ht="31.5">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -4232,7 +5108,7 @@
       <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -4241,17 +5117,23 @@
       <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="63">
+      <c r="K1" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="63">
       <c r="A2" s="4" t="s">
         <v>290</v>
       </c>
@@ -4282,8 +5164,14 @@
       <c r="J2" s="5" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="78.75">
+      <c r="K2" t="s">
+        <v>732</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="94.5">
       <c r="A3" s="4" t="s">
         <v>297</v>
       </c>
@@ -4314,8 +5202,14 @@
       <c r="J3" s="5" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="78.75">
+      <c r="K3" t="s">
+        <v>733</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="94.5">
       <c r="A4" s="4" t="s">
         <v>303</v>
       </c>
@@ -4346,8 +5240,14 @@
       <c r="J4" s="5" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="157.5">
+      <c r="K4" t="s">
+        <v>742</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="157.5">
       <c r="A5" s="4" t="s">
         <v>309</v>
       </c>
@@ -4378,8 +5278,14 @@
       <c r="J5" s="5" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="63">
+      <c r="K5" t="s">
+        <v>734</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="63">
       <c r="A6" s="4" t="s">
         <v>315</v>
       </c>
@@ -4410,8 +5316,14 @@
       <c r="J6" s="5" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="110.25">
+      <c r="K6" t="s">
+        <v>735</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="110.25">
       <c r="A7" s="4" t="s">
         <v>321</v>
       </c>
@@ -4442,8 +5354,14 @@
       <c r="J7" s="5" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="78.75">
+      <c r="K7" t="s">
+        <v>736</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="78.75">
       <c r="A8" s="4" t="s">
         <v>327</v>
       </c>
@@ -4474,8 +5392,14 @@
       <c r="J8" s="5" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="110.25">
+      <c r="K8" t="s">
+        <v>737</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="110.25">
       <c r="A9" s="4" t="s">
         <v>332</v>
       </c>
@@ -4506,8 +5430,14 @@
       <c r="J9" s="5" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="63">
+      <c r="K9" t="s">
+        <v>738</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="63">
       <c r="A10" s="4" t="s">
         <v>338</v>
       </c>
@@ -4538,8 +5468,14 @@
       <c r="J10" s="5" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="110.25">
+      <c r="K10" t="s">
+        <v>739</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="110.25">
       <c r="A11" s="4" t="s">
         <v>344</v>
       </c>
@@ -4570,8 +5506,14 @@
       <c r="J11" s="5" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="47.25">
+      <c r="K11" s="17" t="s">
+        <v>740</v>
+      </c>
+      <c r="L11" s="17" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="47.25">
       <c r="A12" s="4" t="s">
         <v>350</v>
       </c>
@@ -4601,6 +5543,12 @@
       </c>
       <c r="J12" s="5" t="s">
         <v>587</v>
+      </c>
+      <c r="K12" t="s">
+        <v>741</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>753</v>
       </c>
     </row>
   </sheetData>
@@ -4618,7 +5566,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4644,10 +5592,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K17" sqref="F1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4662,9 +5610,11 @@
     <col min="8" max="8" width="70.28515625" customWidth="1"/>
     <col min="9" max="9" width="23.7109375" customWidth="1"/>
     <col min="10" max="10" width="70.28515625" customWidth="1"/>
+    <col min="11" max="11" width="71.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="103.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:12" ht="15.75">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -4695,8 +5645,14 @@
       <c r="J1" s="10" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="94.5">
+      <c r="K1" s="10" t="s">
+        <v>687</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="94.5">
       <c r="A2" s="4" t="s">
         <v>165</v>
       </c>
@@ -4727,8 +5683,14 @@
       <c r="J2" s="5" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="63">
+      <c r="K2" t="s">
+        <v>754</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="63">
       <c r="A3" s="4" t="s">
         <v>172</v>
       </c>
@@ -4759,8 +5721,14 @@
       <c r="J3" s="5" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="94.5">
+      <c r="K3" t="s">
+        <v>755</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="94.5">
       <c r="A4" s="4" t="s">
         <v>178</v>
       </c>
@@ -4791,8 +5759,14 @@
       <c r="J4" s="5" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="47.25">
+      <c r="K4" t="s">
+        <v>756</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="47.25">
       <c r="A5" s="4" t="s">
         <v>184</v>
       </c>
@@ -4823,8 +5797,14 @@
       <c r="J5" s="5" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="141.75">
+      <c r="K5" t="s">
+        <v>757</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="141.75">
       <c r="A6" s="4" t="s">
         <v>190</v>
       </c>
@@ -4855,8 +5835,14 @@
       <c r="J6" s="5" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="31.5">
+      <c r="K6" t="s">
+        <v>758</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="31.5">
       <c r="A7" s="4" t="s">
         <v>195</v>
       </c>
@@ -4887,8 +5873,14 @@
       <c r="J7" s="6" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="47.25">
+      <c r="K7" t="s">
+        <v>759</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="47.25">
       <c r="A8" s="4" t="s">
         <v>201</v>
       </c>
@@ -4908,8 +5900,11 @@
       <c r="I8" s="5" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="31.5">
+      <c r="K8" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="31.5">
       <c r="A9" s="4" t="s">
         <v>204</v>
       </c>
@@ -4931,8 +5926,11 @@
       <c r="I9" s="5" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="189">
+      <c r="K9" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="189">
       <c r="A10" s="4" t="s">
         <v>208</v>
       </c>
@@ -4963,8 +5961,14 @@
       <c r="J10" s="5" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="47.25">
+      <c r="K10" t="s">
+        <v>762</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="47.25">
       <c r="A11" s="4" t="s">
         <v>214</v>
       </c>
@@ -4993,8 +5997,14 @@
       <c r="J11" s="5" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="220.5">
+      <c r="K11" t="s">
+        <v>763</v>
+      </c>
+      <c r="L11" s="17" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="220.5">
       <c r="A12" s="4" t="s">
         <v>218</v>
       </c>
@@ -5025,8 +6035,14 @@
       <c r="J12" s="5" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="31.5">
+      <c r="K12" t="s">
+        <v>764</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="31.5">
       <c r="A13" s="4" t="s">
         <v>224</v>
       </c>
@@ -5046,8 +6062,11 @@
       <c r="I13" s="5" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="47.25">
+      <c r="K13" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="47.25">
       <c r="A14" s="4" t="s">
         <v>227</v>
       </c>
@@ -5067,8 +6086,11 @@
       <c r="I14" s="5" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="31.5">
+      <c r="K14" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="31.5">
       <c r="A15" s="4" t="s">
         <v>230</v>
       </c>
@@ -5090,8 +6112,11 @@
       <c r="I15" s="5" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="47.25">
+      <c r="K15" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="47.25">
       <c r="A16" s="4" t="s">
         <v>234</v>
       </c>
@@ -5120,8 +6145,14 @@
         <v>611</v>
       </c>
       <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" ht="31.5">
+      <c r="K16" t="s">
+        <v>768</v>
+      </c>
+      <c r="L16" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="31.5">
       <c r="A17" s="4" t="s">
         <v>240</v>
       </c>
@@ -5143,8 +6174,11 @@
       <c r="I17" s="5" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="47.25">
+      <c r="K17" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="47.25">
       <c r="A18" s="4" t="s">
         <v>244</v>
       </c>
@@ -5164,8 +6198,11 @@
       <c r="I18" s="5" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="110.25">
+      <c r="K18" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="110.25">
       <c r="A19" s="4" t="s">
         <v>247</v>
       </c>
@@ -5196,8 +6233,14 @@
       <c r="J19" s="5" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="47.25">
+      <c r="K19" t="s">
+        <v>771</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="47.25">
       <c r="A20" s="4" t="s">
         <v>252</v>
       </c>
@@ -5217,8 +6260,11 @@
       <c r="I20" s="5" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="110.25">
+      <c r="K20" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="110.25">
       <c r="A21" s="4" t="s">
         <v>255</v>
       </c>
@@ -5249,8 +6295,14 @@
       <c r="J21" s="5" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="47.25">
+      <c r="K21" t="s">
+        <v>773</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="47.25">
       <c r="A22" s="4" t="s">
         <v>261</v>
       </c>
@@ -5281,8 +6333,14 @@
       <c r="J22" s="4" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="47.25">
+      <c r="K22" t="s">
+        <v>774</v>
+      </c>
+      <c r="L22" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="47.25">
       <c r="A23" s="4" t="s">
         <v>267</v>
       </c>
@@ -5313,8 +6371,14 @@
       <c r="J23" s="5" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="110.25">
+      <c r="K23" t="s">
+        <v>775</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="110.25">
       <c r="A24" s="4" t="s">
         <v>272</v>
       </c>
@@ -5345,8 +6409,14 @@
       <c r="J24" s="5" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="47.25">
+      <c r="K24" t="s">
+        <v>776</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="47.25">
       <c r="A25" s="4" t="s">
         <v>278</v>
       </c>
@@ -5377,8 +6447,14 @@
       <c r="J25" s="5" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="47.25">
+      <c r="K25" t="s">
+        <v>777</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="47.25">
       <c r="A26" s="4" t="s">
         <v>284</v>
       </c>
@@ -5409,8 +6485,14 @@
       <c r="J26" s="5" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75">
+      <c r="K26" t="s">
+        <v>778</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75">
       <c r="G27" s="5"/>
       <c r="I27" s="5"/>
     </row>
@@ -5429,7 +6511,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5455,27 +6537,29 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J12" sqref="B1:J1048576"/>
+    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K1" sqref="E1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+    <col min="5" max="5" width="75.140625" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="52.85546875" customWidth="1"/>
     <col min="8" max="8" width="82" customWidth="1"/>
     <col min="9" max="9" width="41.42578125" customWidth="1"/>
     <col min="10" max="10" width="82" customWidth="1"/>
+    <col min="11" max="11" width="53.28515625" customWidth="1"/>
+    <col min="12" max="12" width="83.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5">
+    <row r="1" spans="1:12" ht="15.75">
       <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
@@ -5506,8 +6590,14 @@
       <c r="J1" s="3" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="110.25">
+      <c r="K1" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="110.25">
       <c r="A2" s="12" t="s">
         <v>356</v>
       </c>
@@ -5538,8 +6628,14 @@
       <c r="J2" s="13" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="157.5">
+      <c r="K2" s="18" t="s">
+        <v>796</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="122.25" customHeight="1">
       <c r="A3" s="12" t="s">
         <v>362</v>
       </c>
@@ -5570,8 +6666,14 @@
       <c r="J3" s="13" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="236.25">
+      <c r="K3" s="18" t="s">
+        <v>797</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="141.75">
       <c r="A4" s="12" t="s">
         <v>367</v>
       </c>
@@ -5602,8 +6704,14 @@
       <c r="J4" s="13" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="267.75">
+      <c r="K4" s="18" t="s">
+        <v>798</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="220.5">
       <c r="A5" s="12" t="s">
         <v>373</v>
       </c>
@@ -5634,8 +6742,14 @@
       <c r="J5" s="13" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="362.25">
+      <c r="K5" s="18" t="s">
+        <v>799</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="247.5" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>378</v>
       </c>
@@ -5666,8 +6780,14 @@
       <c r="J6" s="13" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="299.25">
+      <c r="K6" s="19" t="s">
+        <v>800</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="220.5">
       <c r="A7" s="12" t="s">
         <v>382</v>
       </c>
@@ -5698,8 +6818,14 @@
       <c r="J7" s="13" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="393.75">
+      <c r="K7" s="18" t="s">
+        <v>801</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="240">
       <c r="A8" s="12" t="s">
         <v>388</v>
       </c>
@@ -5730,8 +6856,14 @@
       <c r="J8" s="13" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="94.5">
+      <c r="K8" s="12" t="s">
+        <v>817</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="78.75">
       <c r="A9" s="12" t="s">
         <v>394</v>
       </c>
@@ -5762,8 +6894,14 @@
       <c r="J9" s="13" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="31.5">
+      <c r="K9" s="18" t="s">
+        <v>816</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="31.5">
       <c r="A10" s="12" t="s">
         <v>400</v>
       </c>
@@ -5785,8 +6923,11 @@
       <c r="I10" s="12" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="31.5">
+      <c r="K10" s="18" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="31.5">
       <c r="A11" s="12" t="s">
         <v>404</v>
       </c>
@@ -5808,8 +6949,11 @@
       <c r="I11" s="12" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="94.5">
+      <c r="K11" s="18" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="63">
       <c r="A12" s="12" t="s">
         <v>407</v>
       </c>
@@ -5840,8 +6984,14 @@
       <c r="J12" s="13" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="110.25">
+      <c r="K12" t="s">
+        <v>818</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="78.75">
       <c r="A13" s="12" t="s">
         <v>412</v>
       </c>
@@ -5872,8 +7022,14 @@
       <c r="J13" s="13" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="47.25">
+      <c r="K13" t="s">
+        <v>819</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="31.5">
       <c r="A14" s="12" t="s">
         <v>417</v>
       </c>
@@ -5904,8 +7060,14 @@
       <c r="J14" s="13" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75">
+      <c r="K14" s="18" t="s">
+        <v>803</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="12" t="s">
         <v>423</v>
       </c>
@@ -5936,8 +7098,14 @@
       <c r="J15" s="12" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="63">
+      <c r="K15" s="18" t="s">
+        <v>820</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="47.25">
       <c r="A16" s="12" t="s">
         <v>429</v>
       </c>
@@ -5968,8 +7136,14 @@
       <c r="J16" s="13" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75">
+      <c r="K16" s="18" t="s">
+        <v>821</v>
+      </c>
+      <c r="L16" s="17" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="12" t="s">
         <v>436</v>
       </c>
@@ -6000,8 +7174,14 @@
       <c r="J17" s="12" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="63">
+      <c r="K17" s="18" t="s">
+        <v>822</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="47.25">
       <c r="A18" s="12" t="s">
         <v>441</v>
       </c>
@@ -6032,8 +7212,14 @@
       <c r="J18" s="13" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="63">
+      <c r="K18" s="18" t="s">
+        <v>804</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="47.25">
       <c r="A19" s="12" t="s">
         <v>446</v>
       </c>
@@ -6064,8 +7250,14 @@
       <c r="J19" s="13" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="47.25">
+      <c r="K19" s="18" t="s">
+        <v>805</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="31.5">
       <c r="A20" s="12" t="s">
         <v>452</v>
       </c>
@@ -6096,8 +7288,14 @@
       <c r="J20" s="13" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="47.25">
+      <c r="K20" s="18" t="s">
+        <v>806</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="31.5">
       <c r="A21" s="12" t="s">
         <v>458</v>
       </c>
@@ -6128,8 +7326,14 @@
       <c r="J21" s="13" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="47.25">
+      <c r="K21" s="18" t="s">
+        <v>807</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="31.5">
       <c r="A22" s="13" t="s">
         <v>464</v>
       </c>
@@ -6160,8 +7364,14 @@
       <c r="J22" s="13" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="31.5">
+      <c r="K22" s="18" t="s">
+        <v>808</v>
+      </c>
+      <c r="L22" s="17" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75">
       <c r="A23" s="15" t="s">
         <v>469</v>
       </c>
@@ -6192,8 +7402,14 @@
       <c r="J23" s="13" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="31.5">
+      <c r="K23" s="18" t="s">
+        <v>809</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="31.5">
       <c r="A24" s="13" t="s">
         <v>474</v>
       </c>
@@ -6224,8 +7440,14 @@
       <c r="J24" s="13" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="78.75">
+      <c r="K24" s="18" t="s">
+        <v>475</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="63">
       <c r="A25" s="12" t="s">
         <v>478</v>
       </c>
@@ -6256,8 +7478,14 @@
       <c r="J25" s="13" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="110.25">
+      <c r="K25" s="18" t="s">
+        <v>810</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="63">
       <c r="A26" s="13" t="s">
         <v>483</v>
       </c>
@@ -6288,8 +7516,14 @@
       <c r="J26" s="13" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="47.25">
+      <c r="K26" s="18" t="s">
+        <v>811</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="31.5">
       <c r="A27" s="12" t="s">
         <v>489</v>
       </c>
@@ -6320,8 +7554,14 @@
       <c r="J27" s="13" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="47.25">
+      <c r="K27" s="18" t="s">
+        <v>812</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="31.5">
       <c r="A28" s="12" t="s">
         <v>495</v>
       </c>
@@ -6352,8 +7592,14 @@
       <c r="J28" s="13" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="47.25">
+      <c r="K28" s="18" t="s">
+        <v>813</v>
+      </c>
+      <c r="L28" s="17" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="54.75" customHeight="1">
       <c r="A29" s="12" t="s">
         <v>500</v>
       </c>
@@ -6384,8 +7630,14 @@
       <c r="J29" s="13" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="63">
+      <c r="K29" s="18" t="s">
+        <v>814</v>
+      </c>
+      <c r="L29" s="17" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="47.25">
       <c r="A30" s="13" t="s">
         <v>506</v>
       </c>
@@ -6416,8 +7668,14 @@
       <c r="J30" s="13" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="63">
+      <c r="K30" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="L30" s="17" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="47.25">
       <c r="A31" s="12" t="s">
         <v>511</v>
       </c>
@@ -6448,8 +7706,14 @@
       <c r="J31" s="13" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="94.5">
+      <c r="K31" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="63">
       <c r="A32" s="12" t="s">
         <v>515</v>
       </c>
@@ -6479,6 +7743,12 @@
       </c>
       <c r="J32" s="13" t="s">
         <v>682</v>
+      </c>
+      <c r="K32" s="18" t="s">
+        <v>815</v>
+      </c>
+      <c r="L32" s="17" t="s">
+        <v>848</v>
       </c>
     </row>
   </sheetData>

</xml_diff>